<commit_message>
changed name from grafiken to assets
</commit_message>
<xml_diff>
--- a/doc/Projektplan Gantt.xlsx
+++ b/doc/Projektplan Gantt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-435" windowWidth="25605" windowHeight="16005"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="25610" windowHeight="16010"/>
   </bookViews>
   <sheets>
     <sheet name="Balkenplan" sheetId="1" r:id="rId1"/>
@@ -113,9 +113,6 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>Grafiken Erstellen und Einbinden</t>
-  </si>
-  <si>
     <t>Gamelogik:  Erfolg Liste</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>Dauer in Total h</t>
+  </si>
+  <si>
+    <t>Assets Erstellen und Einbinden</t>
   </si>
 </sst>
 </file>
@@ -716,17 +716,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -735,15 +729,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -755,8 +740,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -775,6 +766,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="69">
@@ -1283,73 +1283,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="81" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.140625" style="5" customWidth="1"/>
-    <col min="7" max="8" width="3.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="3.140625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="3.140625" style="5" customWidth="1"/>
-    <col min="11" max="12" width="3.140625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="8" customWidth="1"/>
-    <col min="14" max="14" width="3.140625" style="5" customWidth="1"/>
-    <col min="15" max="16" width="3.140625" style="6" customWidth="1"/>
-    <col min="17" max="17" width="3.140625" style="8" customWidth="1"/>
-    <col min="18" max="18" width="3.140625" style="5" customWidth="1"/>
-    <col min="19" max="20" width="3.140625" style="6" customWidth="1"/>
-    <col min="21" max="21" width="3.140625" style="8" customWidth="1"/>
-    <col min="22" max="22" width="3.140625" style="5" customWidth="1"/>
-    <col min="23" max="24" width="3.140625" style="6" customWidth="1"/>
-    <col min="25" max="25" width="3.140625" style="8" customWidth="1"/>
-    <col min="26" max="26" width="3.140625" style="5" customWidth="1"/>
-    <col min="27" max="28" width="3.140625" style="6" customWidth="1"/>
-    <col min="29" max="29" width="3.140625" style="8" customWidth="1"/>
-    <col min="30" max="30" width="3.140625" style="5" customWidth="1"/>
-    <col min="31" max="32" width="3.140625" style="6" customWidth="1"/>
-    <col min="33" max="33" width="3.140625" style="8" customWidth="1"/>
-    <col min="34" max="34" width="3.140625" style="5" customWidth="1"/>
-    <col min="35" max="36" width="3.140625" style="6" customWidth="1"/>
-    <col min="37" max="37" width="3.140625" style="8" customWidth="1"/>
-    <col min="38" max="38" width="3.140625" style="5" customWidth="1"/>
-    <col min="39" max="40" width="3.140625" style="6" customWidth="1"/>
-    <col min="41" max="41" width="3.140625" style="8" customWidth="1"/>
-    <col min="42" max="42" width="3.140625" style="5" customWidth="1"/>
-    <col min="43" max="44" width="3.140625" style="6" customWidth="1"/>
-    <col min="45" max="45" width="3.140625" style="8" customWidth="1"/>
-    <col min="46" max="46" width="3.140625" style="5" customWidth="1"/>
-    <col min="47" max="48" width="3.140625" style="6" customWidth="1"/>
-    <col min="49" max="49" width="3.140625" style="8" customWidth="1"/>
-    <col min="50" max="50" width="3.140625" style="5" customWidth="1"/>
-    <col min="51" max="52" width="3.140625" style="6" customWidth="1"/>
-    <col min="53" max="53" width="3.140625" style="8" customWidth="1"/>
-    <col min="54" max="54" width="3.140625" style="5" customWidth="1"/>
-    <col min="55" max="56" width="3.140625" style="6" customWidth="1"/>
-    <col min="57" max="57" width="3.140625" style="8" customWidth="1"/>
-    <col min="58" max="58" width="3.140625" style="5" customWidth="1"/>
-    <col min="59" max="60" width="3.140625" style="6" customWidth="1"/>
-    <col min="61" max="61" width="3.140625" style="8" customWidth="1"/>
-    <col min="62" max="62" width="3.140625" style="5" customWidth="1"/>
-    <col min="63" max="64" width="3.140625" style="6" customWidth="1"/>
-    <col min="65" max="65" width="3.140625" style="8" customWidth="1"/>
-    <col min="66" max="66" width="3.140625" style="5" customWidth="1"/>
-    <col min="67" max="68" width="3.140625" style="6" customWidth="1"/>
-    <col min="69" max="69" width="3.140625" style="8" customWidth="1"/>
-    <col min="70" max="70" width="3.140625" style="5" customWidth="1"/>
-    <col min="71" max="71" width="2.7109375" customWidth="1"/>
-    <col min="72" max="72" width="2.42578125" customWidth="1"/>
-    <col min="73" max="73" width="2.140625" customWidth="1"/>
-    <col min="74" max="74" width="2.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7265625" customWidth="1"/>
+    <col min="3" max="4" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="4.453125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.1796875" style="5" customWidth="1"/>
+    <col min="7" max="8" width="3.1796875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="3.1796875" style="8" customWidth="1"/>
+    <col min="10" max="10" width="3.1796875" style="5" customWidth="1"/>
+    <col min="11" max="12" width="3.1796875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="3.1796875" style="8" customWidth="1"/>
+    <col min="14" max="14" width="3.1796875" style="5" customWidth="1"/>
+    <col min="15" max="16" width="3.1796875" style="6" customWidth="1"/>
+    <col min="17" max="17" width="3.1796875" style="8" customWidth="1"/>
+    <col min="18" max="18" width="3.1796875" style="5" customWidth="1"/>
+    <col min="19" max="20" width="3.1796875" style="6" customWidth="1"/>
+    <col min="21" max="21" width="3.1796875" style="8" customWidth="1"/>
+    <col min="22" max="22" width="3.1796875" style="5" customWidth="1"/>
+    <col min="23" max="24" width="3.1796875" style="6" customWidth="1"/>
+    <col min="25" max="25" width="3.1796875" style="8" customWidth="1"/>
+    <col min="26" max="26" width="3.1796875" style="5" customWidth="1"/>
+    <col min="27" max="28" width="3.1796875" style="6" customWidth="1"/>
+    <col min="29" max="29" width="3.1796875" style="8" customWidth="1"/>
+    <col min="30" max="30" width="3.1796875" style="5" customWidth="1"/>
+    <col min="31" max="32" width="3.1796875" style="6" customWidth="1"/>
+    <col min="33" max="33" width="3.1796875" style="8" customWidth="1"/>
+    <col min="34" max="34" width="3.1796875" style="5" customWidth="1"/>
+    <col min="35" max="36" width="3.1796875" style="6" customWidth="1"/>
+    <col min="37" max="37" width="3.1796875" style="8" customWidth="1"/>
+    <col min="38" max="38" width="3.1796875" style="5" customWidth="1"/>
+    <col min="39" max="40" width="3.1796875" style="6" customWidth="1"/>
+    <col min="41" max="41" width="3.1796875" style="8" customWidth="1"/>
+    <col min="42" max="42" width="3.1796875" style="5" customWidth="1"/>
+    <col min="43" max="44" width="3.1796875" style="6" customWidth="1"/>
+    <col min="45" max="45" width="3.1796875" style="8" customWidth="1"/>
+    <col min="46" max="46" width="3.1796875" style="5" customWidth="1"/>
+    <col min="47" max="48" width="3.1796875" style="6" customWidth="1"/>
+    <col min="49" max="49" width="3.1796875" style="8" customWidth="1"/>
+    <col min="50" max="50" width="3.1796875" style="5" customWidth="1"/>
+    <col min="51" max="52" width="3.1796875" style="6" customWidth="1"/>
+    <col min="53" max="53" width="3.1796875" style="8" customWidth="1"/>
+    <col min="54" max="54" width="3.1796875" style="5" customWidth="1"/>
+    <col min="55" max="56" width="3.1796875" style="6" customWidth="1"/>
+    <col min="57" max="57" width="3.1796875" style="8" customWidth="1"/>
+    <col min="58" max="58" width="3.1796875" style="5" customWidth="1"/>
+    <col min="59" max="60" width="3.1796875" style="6" customWidth="1"/>
+    <col min="61" max="61" width="3.1796875" style="8" customWidth="1"/>
+    <col min="62" max="62" width="3.1796875" style="5" customWidth="1"/>
+    <col min="63" max="64" width="3.1796875" style="6" customWidth="1"/>
+    <col min="65" max="65" width="3.1796875" style="8" customWidth="1"/>
+    <col min="66" max="66" width="3.1796875" style="5" customWidth="1"/>
+    <col min="67" max="68" width="3.1796875" style="6" customWidth="1"/>
+    <col min="69" max="69" width="3.1796875" style="8" customWidth="1"/>
+    <col min="70" max="70" width="3.1796875" style="5" customWidth="1"/>
+    <col min="71" max="71" width="2.7265625" customWidth="1"/>
+    <col min="72" max="72" width="2.453125" customWidth="1"/>
+    <col min="73" max="73" width="2.1796875" customWidth="1"/>
+    <col min="74" max="74" width="2.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:72" s="2" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="75" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="26"/>
@@ -1358,111 +1358,111 @@
         <v>3</v>
       </c>
       <c r="E1" s="35"/>
-      <c r="F1" s="56">
+      <c r="F1" s="64">
         <v>42031</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="56">
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="64">
         <v>42038</v>
       </c>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="56">
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="64">
         <v>42045</v>
       </c>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="56">
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="64">
         <v>42052</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="56">
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="64">
         <v>42059</v>
       </c>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="58"/>
-      <c r="Z1" s="56">
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="64">
         <v>42066</v>
       </c>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="57"/>
-      <c r="AC1" s="58"/>
-      <c r="AD1" s="56">
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="64">
         <v>42073</v>
       </c>
-      <c r="AE1" s="57"/>
-      <c r="AF1" s="57"/>
-      <c r="AG1" s="58"/>
-      <c r="AH1" s="56">
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="64">
         <v>42080</v>
       </c>
-      <c r="AI1" s="57"/>
-      <c r="AJ1" s="57"/>
-      <c r="AK1" s="58"/>
-      <c r="AL1" s="56">
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="66"/>
+      <c r="AL1" s="64">
         <v>42087</v>
       </c>
-      <c r="AM1" s="57"/>
-      <c r="AN1" s="57"/>
-      <c r="AO1" s="58"/>
-      <c r="AP1" s="56">
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="66"/>
+      <c r="AP1" s="64">
         <v>42115</v>
       </c>
-      <c r="AQ1" s="57"/>
-      <c r="AR1" s="57"/>
-      <c r="AS1" s="58"/>
-      <c r="AT1" s="56">
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="65"/>
+      <c r="AS1" s="66"/>
+      <c r="AT1" s="64">
         <v>42122</v>
       </c>
-      <c r="AU1" s="57"/>
-      <c r="AV1" s="57"/>
-      <c r="AW1" s="58"/>
-      <c r="AX1" s="56">
+      <c r="AU1" s="65"/>
+      <c r="AV1" s="65"/>
+      <c r="AW1" s="66"/>
+      <c r="AX1" s="64">
         <v>42129</v>
       </c>
-      <c r="AY1" s="57"/>
-      <c r="AZ1" s="57"/>
-      <c r="BA1" s="58"/>
-      <c r="BB1" s="56">
+      <c r="AY1" s="65"/>
+      <c r="AZ1" s="65"/>
+      <c r="BA1" s="66"/>
+      <c r="BB1" s="64">
         <v>42136</v>
       </c>
-      <c r="BC1" s="57"/>
-      <c r="BD1" s="57"/>
-      <c r="BE1" s="58"/>
-      <c r="BF1" s="56">
+      <c r="BC1" s="65"/>
+      <c r="BD1" s="65"/>
+      <c r="BE1" s="66"/>
+      <c r="BF1" s="64">
         <v>42143</v>
       </c>
-      <c r="BG1" s="57"/>
-      <c r="BH1" s="57"/>
-      <c r="BI1" s="58"/>
-      <c r="BJ1" s="56">
+      <c r="BG1" s="65"/>
+      <c r="BH1" s="65"/>
+      <c r="BI1" s="66"/>
+      <c r="BJ1" s="64">
         <v>42150</v>
       </c>
-      <c r="BK1" s="57"/>
-      <c r="BL1" s="57"/>
-      <c r="BM1" s="58"/>
-      <c r="BN1" s="56">
+      <c r="BK1" s="65"/>
+      <c r="BL1" s="65"/>
+      <c r="BM1" s="66"/>
+      <c r="BN1" s="64">
         <v>42157</v>
       </c>
-      <c r="BO1" s="57"/>
-      <c r="BP1" s="57"/>
-      <c r="BQ1" s="58"/>
+      <c r="BO1" s="65"/>
+      <c r="BP1" s="65"/>
+      <c r="BQ1" s="66"/>
       <c r="BR1" s="9"/>
     </row>
-    <row r="2" spans="1:72" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59"/>
+    <row r="2" spans="1:72" s="1" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="75"/>
       <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="36"/>
@@ -1662,17 +1662,17 @@
       <c r="BS2" s="4"/>
       <c r="BT2" s="4"/>
     </row>
-    <row r="3" spans="1:72" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:72" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="55">
         <v>1</v>
       </c>
-      <c r="B3" s="70" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="64">
+      <c r="B3" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="56">
         <v>4</v>
       </c>
-      <c r="D3" s="64"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="38" t="s">
         <v>1</v>
       </c>
@@ -1714,11 +1714,11 @@
       <c r="BQ3" s="12"/>
       <c r="BR3" s="10"/>
     </row>
-    <row r="4" spans="1:72" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:72" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="55"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="39" t="s">
         <v>2</v>
       </c>
@@ -1788,17 +1788,17 @@
       <c r="BQ4" s="15"/>
       <c r="BR4" s="13"/>
     </row>
-    <row r="5" spans="1:72" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:72" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="55">
         <v>2</v>
       </c>
-      <c r="B5" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="62">
+      <c r="B5" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="60">
         <v>4</v>
       </c>
-      <c r="D5" s="60"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="31" t="s">
         <v>1</v>
       </c>
@@ -1841,11 +1841,11 @@
       <c r="BQ5" s="19"/>
       <c r="BR5" s="17"/>
     </row>
-    <row r="6" spans="1:72" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:72" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="55"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
       <c r="E6" s="32" t="s">
         <v>2</v>
       </c>
@@ -1915,17 +1915,17 @@
       <c r="BQ6" s="22"/>
       <c r="BR6" s="20"/>
     </row>
-    <row r="7" spans="1:72" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:72" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="55">
         <v>3</v>
       </c>
-      <c r="B7" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="66">
+      <c r="B7" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="61">
         <v>4</v>
       </c>
-      <c r="D7" s="67"/>
+      <c r="D7" s="62"/>
       <c r="E7" s="29" t="s">
         <v>1</v>
       </c>
@@ -1968,11 +1968,11 @@
       <c r="BQ7" s="12"/>
       <c r="BR7" s="10"/>
     </row>
-    <row r="8" spans="1:72" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:72" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="55"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="68"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="63"/>
       <c r="E8" s="30" t="s">
         <v>2</v>
       </c>
@@ -2042,17 +2042,17 @@
       <c r="BQ8" s="15"/>
       <c r="BR8" s="13"/>
     </row>
-    <row r="9" spans="1:72" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:72" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="55">
         <v>7</v>
       </c>
-      <c r="B9" s="60" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="62">
+      <c r="B9" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="60">
         <v>6</v>
       </c>
-      <c r="D9" s="60"/>
+      <c r="D9" s="58"/>
       <c r="E9" s="31" t="s">
         <v>1</v>
       </c>
@@ -2097,11 +2097,11 @@
       <c r="BQ9" s="19"/>
       <c r="BR9" s="17"/>
     </row>
-    <row r="10" spans="1:72" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:72" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="55"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
       <c r="E10" s="32" t="s">
         <v>2</v>
       </c>
@@ -2171,17 +2171,17 @@
       <c r="BQ10" s="22"/>
       <c r="BR10" s="20"/>
     </row>
-    <row r="11" spans="1:72" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:72" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="55">
         <v>4</v>
       </c>
-      <c r="B11" s="64" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="66">
-        <v>1</v>
-      </c>
-      <c r="D11" s="67"/>
+      <c r="B11" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="61">
+        <v>1</v>
+      </c>
+      <c r="D11" s="62"/>
       <c r="E11" s="29" t="s">
         <v>1</v>
       </c>
@@ -2222,11 +2222,11 @@
       <c r="BQ11" s="12"/>
       <c r="BR11" s="10"/>
     </row>
-    <row r="12" spans="1:72" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:72" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="55"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="68"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="63"/>
       <c r="E12" s="30" t="s">
         <v>2</v>
       </c>
@@ -2296,17 +2296,17 @@
       <c r="BQ12" s="15"/>
       <c r="BR12" s="13"/>
     </row>
-    <row r="13" spans="1:72" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:72" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="55">
         <v>5</v>
       </c>
-      <c r="B13" s="60" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="60">
+      <c r="B13" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="58">
         <v>4</v>
       </c>
-      <c r="D13" s="60"/>
+      <c r="D13" s="58"/>
       <c r="E13" s="31" t="s">
         <v>1</v>
       </c>
@@ -2349,11 +2349,11 @@
       <c r="BQ13" s="19"/>
       <c r="BR13" s="17"/>
     </row>
-    <row r="14" spans="1:72" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:72" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="55"/>
-      <c r="B14" s="69"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
       <c r="E14" s="32" t="s">
         <v>2</v>
       </c>
@@ -2423,17 +2423,17 @@
       <c r="BQ14" s="22"/>
       <c r="BR14" s="20"/>
     </row>
-    <row r="15" spans="1:72" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:72" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="55">
         <v>6</v>
       </c>
-      <c r="B15" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="64">
+      <c r="B15" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="56">
         <v>3</v>
       </c>
-      <c r="D15" s="64"/>
+      <c r="D15" s="56"/>
       <c r="E15" s="29" t="s">
         <v>1</v>
       </c>
@@ -2476,11 +2476,11 @@
       <c r="BQ15" s="12"/>
       <c r="BR15" s="10"/>
     </row>
-    <row r="16" spans="1:72" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:72" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="55"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="30" t="s">
         <v>2</v>
       </c>
@@ -2550,17 +2550,17 @@
       <c r="BQ16" s="15"/>
       <c r="BR16" s="13"/>
     </row>
-    <row r="17" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="55">
         <v>7</v>
       </c>
-      <c r="B17" s="60" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="62">
+      <c r="B17" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="60">
         <v>4</v>
       </c>
-      <c r="D17" s="60"/>
+      <c r="D17" s="58"/>
       <c r="E17" s="31" t="s">
         <v>1</v>
       </c>
@@ -2603,11 +2603,11 @@
       <c r="BQ17" s="19"/>
       <c r="BR17" s="17"/>
     </row>
-    <row r="18" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="55"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
       <c r="E18" s="32" t="s">
         <v>2</v>
       </c>
@@ -2677,17 +2677,17 @@
       <c r="BQ18" s="22"/>
       <c r="BR18" s="20"/>
     </row>
-    <row r="19" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="55">
         <v>8</v>
       </c>
       <c r="B19" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="64">
+      <c r="C19" s="56">
         <v>8</v>
       </c>
-      <c r="D19" s="64"/>
+      <c r="D19" s="56"/>
       <c r="E19" s="29" t="s">
         <v>1</v>
       </c>
@@ -2735,13 +2735,13 @@
       <c r="BQ19" s="12"/>
       <c r="BR19" s="10"/>
     </row>
-    <row r="20" spans="1:70" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:70" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="55"/>
       <c r="B20" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="30" t="s">
         <v>2</v>
       </c>
@@ -2811,17 +2811,17 @@
       <c r="BQ20" s="15"/>
       <c r="BR20" s="13"/>
     </row>
-    <row r="21" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="55">
         <v>7</v>
       </c>
-      <c r="B21" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="62">
+      <c r="B21" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="60">
         <v>4</v>
       </c>
-      <c r="D21" s="60"/>
+      <c r="D21" s="58"/>
       <c r="E21" s="31" t="s">
         <v>1</v>
       </c>
@@ -2864,11 +2864,11 @@
       <c r="BQ21" s="19"/>
       <c r="BR21" s="17"/>
     </row>
-    <row r="22" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="55"/>
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
       <c r="E22" s="32" t="s">
         <v>2</v>
       </c>
@@ -2938,17 +2938,17 @@
       <c r="BQ22" s="22"/>
       <c r="BR22" s="20"/>
     </row>
-    <row r="23" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="55">
         <v>8</v>
       </c>
-      <c r="B23" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="64">
+      <c r="B23" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="56">
         <v>4</v>
       </c>
-      <c r="D23" s="64"/>
+      <c r="D23" s="56"/>
       <c r="E23" s="29" t="s">
         <v>1</v>
       </c>
@@ -2991,11 +2991,11 @@
       <c r="BQ23" s="12"/>
       <c r="BR23" s="10"/>
     </row>
-    <row r="24" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="55"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
       <c r="E24" s="30" t="s">
         <v>2</v>
       </c>
@@ -3065,17 +3065,17 @@
       <c r="BQ24" s="15"/>
       <c r="BR24" s="13"/>
     </row>
-    <row r="25" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="55">
         <v>7</v>
       </c>
-      <c r="B25" s="60" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="62">
+      <c r="B25" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="60">
         <v>4</v>
       </c>
-      <c r="D25" s="60"/>
+      <c r="D25" s="58"/>
       <c r="E25" s="31" t="s">
         <v>1</v>
       </c>
@@ -3118,11 +3118,11 @@
       <c r="BQ25" s="19"/>
       <c r="BR25" s="17"/>
     </row>
-    <row r="26" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="55"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
       <c r="E26" s="32" t="s">
         <v>2</v>
       </c>
@@ -3192,17 +3192,17 @@
       <c r="BQ26" s="22"/>
       <c r="BR26" s="20"/>
     </row>
-    <row r="27" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="55">
         <v>8</v>
       </c>
-      <c r="B27" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="64">
+      <c r="B27" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="56">
         <v>4</v>
       </c>
-      <c r="D27" s="64"/>
+      <c r="D27" s="56"/>
       <c r="E27" s="29" t="s">
         <v>1</v>
       </c>
@@ -3245,11 +3245,11 @@
       <c r="BQ27" s="12"/>
       <c r="BR27" s="10"/>
     </row>
-    <row r="28" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="55"/>
-      <c r="B28" s="65"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="65"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
       <c r="E28" s="30" t="s">
         <v>2</v>
       </c>
@@ -3319,17 +3319,17 @@
       <c r="BQ28" s="15"/>
       <c r="BR28" s="13"/>
     </row>
-    <row r="29" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="55">
         <v>9</v>
       </c>
-      <c r="B29" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="60">
+      <c r="B29" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="58">
         <v>12</v>
       </c>
-      <c r="D29" s="60"/>
+      <c r="D29" s="58"/>
       <c r="E29" s="31" t="s">
         <v>1</v>
       </c>
@@ -3397,11 +3397,11 @@
       <c r="BQ29" s="19"/>
       <c r="BR29" s="17"/>
     </row>
-    <row r="30" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="55"/>
-      <c r="B30" s="61"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
       <c r="E30" s="32" t="s">
         <v>2</v>
       </c>
@@ -3471,17 +3471,17 @@
       <c r="BQ30" s="22"/>
       <c r="BR30" s="20"/>
     </row>
-    <row r="31" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="55">
         <v>10</v>
       </c>
-      <c r="B31" s="64" t="s">
+      <c r="B31" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="64">
+      <c r="C31" s="56">
         <v>8</v>
       </c>
-      <c r="D31" s="64"/>
+      <c r="D31" s="56"/>
       <c r="E31" s="29" t="s">
         <v>1</v>
       </c>
@@ -3529,11 +3529,11 @@
       <c r="BQ31" s="12"/>
       <c r="BR31" s="10"/>
     </row>
-    <row r="32" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="55"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
       <c r="E32" s="30" t="s">
         <v>2</v>
       </c>
@@ -3603,17 +3603,17 @@
       <c r="BQ32" s="15"/>
       <c r="BR32" s="13"/>
     </row>
-    <row r="33" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="55">
         <v>11</v>
       </c>
-      <c r="B33" s="60" t="s">
+      <c r="B33" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="60">
+      <c r="C33" s="58">
         <v>8</v>
       </c>
-      <c r="D33" s="60"/>
+      <c r="D33" s="58"/>
       <c r="E33" s="31" t="s">
         <v>1</v>
       </c>
@@ -3701,11 +3701,11 @@
       <c r="BQ33" s="19"/>
       <c r="BR33" s="17"/>
     </row>
-    <row r="34" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="55"/>
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
       <c r="E34" s="32" t="s">
         <v>2</v>
       </c>
@@ -3775,17 +3775,17 @@
       <c r="BQ34" s="22"/>
       <c r="BR34" s="20"/>
     </row>
-    <row r="35" spans="1:70" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:70" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="55">
         <v>12</v>
       </c>
-      <c r="B35" s="70" t="s">
+      <c r="B35" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="64">
+      <c r="C35" s="56">
         <v>2</v>
       </c>
-      <c r="D35" s="64"/>
+      <c r="D35" s="56"/>
       <c r="E35" s="29" t="s">
         <v>1</v>
       </c>
@@ -3825,11 +3825,11 @@
       <c r="BQ35" s="12"/>
       <c r="BR35" s="10"/>
     </row>
-    <row r="36" spans="1:70" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:70" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="55"/>
-      <c r="B36" s="71"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="65"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
       <c r="E36" s="30" t="s">
         <v>2</v>
       </c>
@@ -3899,17 +3899,17 @@
       <c r="BQ36" s="15"/>
       <c r="BR36" s="13"/>
     </row>
-    <row r="37" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="55">
         <v>13</v>
       </c>
-      <c r="B37" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="60">
+      <c r="B37" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="58">
         <v>6</v>
       </c>
-      <c r="D37" s="60"/>
+      <c r="D37" s="58"/>
       <c r="E37" s="31" t="s">
         <v>1</v>
       </c>
@@ -3960,11 +3960,11 @@
       <c r="BQ37" s="19"/>
       <c r="BR37" s="17"/>
     </row>
-    <row r="38" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="55"/>
-      <c r="B38" s="61"/>
-      <c r="C38" s="61"/>
-      <c r="D38" s="61"/>
+      <c r="B38" s="59"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
       <c r="E38" s="32" t="s">
         <v>2</v>
       </c>
@@ -4034,17 +4034,17 @@
       <c r="BQ38" s="22"/>
       <c r="BR38" s="20"/>
     </row>
-    <row r="39" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="55">
         <v>14</v>
       </c>
-      <c r="B39" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="64">
+      <c r="B39" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="56">
         <v>4</v>
       </c>
-      <c r="D39" s="64"/>
+      <c r="D39" s="56"/>
       <c r="E39" s="29" t="s">
         <v>1</v>
       </c>
@@ -4092,11 +4092,11 @@
       <c r="BQ39" s="12"/>
       <c r="BR39" s="10"/>
     </row>
-    <row r="40" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="55"/>
-      <c r="B40" s="65"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="65"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="57"/>
       <c r="E40" s="30" t="s">
         <v>2</v>
       </c>
@@ -4166,13 +4166,13 @@
       <c r="BQ40" s="15"/>
       <c r="BR40" s="13"/>
     </row>
-    <row r="41" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="55">
         <v>15</v>
       </c>
-      <c r="B41" s="60"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="58"/>
       <c r="E41" s="31" t="s">
         <v>1</v>
       </c>
@@ -4210,11 +4210,11 @@
       <c r="BQ41" s="19"/>
       <c r="BR41" s="17"/>
     </row>
-    <row r="42" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="55"/>
-      <c r="B42" s="61"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="61"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
       <c r="E42" s="32" t="s">
         <v>2</v>
       </c>
@@ -4284,7 +4284,7 @@
       <c r="BQ42" s="22"/>
       <c r="BR42" s="20"/>
     </row>
-    <row r="43" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="55">
         <v>16</v>
       </c>
@@ -4328,7 +4328,7 @@
       <c r="BQ43" s="12"/>
       <c r="BR43" s="10"/>
     </row>
-    <row r="44" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="55"/>
       <c r="B44" s="50"/>
       <c r="C44" s="52"/>
@@ -4402,15 +4402,15 @@
       <c r="BQ44" s="15"/>
       <c r="BR44" s="13"/>
     </row>
-    <row r="45" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="55">
         <v>18</v>
       </c>
-      <c r="B45" s="72" t="s">
+      <c r="B45" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="74"/>
-      <c r="D45" s="74"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="71"/>
       <c r="E45" s="40"/>
       <c r="F45" s="41"/>
       <c r="G45" s="42"/>
@@ -4498,11 +4498,11 @@
       <c r="BQ45" s="43"/>
       <c r="BR45" s="10"/>
     </row>
-    <row r="46" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="55"/>
-      <c r="B46" s="73"/>
-      <c r="C46" s="75"/>
-      <c r="D46" s="75"/>
+      <c r="B46" s="70"/>
+      <c r="C46" s="72"/>
+      <c r="D46" s="72"/>
       <c r="E46" s="44"/>
       <c r="F46" s="45"/>
       <c r="G46" s="46"/>
@@ -4570,15 +4570,15 @@
       <c r="BQ46" s="47"/>
       <c r="BR46" s="13"/>
     </row>
-    <row r="47" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="55">
         <v>19</v>
       </c>
-      <c r="B47" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47" s="60"/>
-      <c r="D47" s="60"/>
+      <c r="B47" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
       <c r="E47" s="31"/>
       <c r="F47" s="17"/>
       <c r="I47" s="19"/>
@@ -4614,11 +4614,11 @@
       <c r="BQ47" s="19"/>
       <c r="BR47" s="17"/>
     </row>
-    <row r="48" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="55"/>
-      <c r="B48" s="61"/>
-      <c r="C48" s="61"/>
-      <c r="D48" s="61"/>
+      <c r="B48" s="59"/>
+      <c r="C48" s="59"/>
+      <c r="D48" s="59"/>
       <c r="E48" s="32"/>
       <c r="F48" s="20"/>
       <c r="G48" s="21"/>
@@ -4686,15 +4686,15 @@
       <c r="BQ48" s="22"/>
       <c r="BR48" s="20"/>
     </row>
-    <row r="49" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="55">
         <v>20</v>
       </c>
-      <c r="B49" s="64" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" s="64"/>
-      <c r="D49" s="64"/>
+      <c r="B49" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="56"/>
+      <c r="D49" s="56"/>
       <c r="E49" s="29"/>
       <c r="F49" s="10"/>
       <c r="I49" s="12"/>
@@ -4730,11 +4730,11 @@
       <c r="BQ49" s="12"/>
       <c r="BR49" s="10"/>
     </row>
-    <row r="50" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="55"/>
-      <c r="B50" s="65"/>
-      <c r="C50" s="65"/>
-      <c r="D50" s="65"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
       <c r="E50" s="30"/>
       <c r="F50" s="13"/>
       <c r="G50" s="14"/>
@@ -4802,15 +4802,15 @@
       <c r="BQ50" s="15"/>
       <c r="BR50" s="13"/>
     </row>
-    <row r="51" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="55">
         <v>21</v>
       </c>
-      <c r="B51" s="60" t="s">
-        <v>43</v>
-      </c>
-      <c r="C51" s="60"/>
-      <c r="D51" s="60"/>
+      <c r="B51" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="58"/>
+      <c r="D51" s="58"/>
       <c r="E51" s="31"/>
       <c r="F51" s="17"/>
       <c r="I51" s="19"/>
@@ -4846,11 +4846,11 @@
       <c r="BQ51" s="19"/>
       <c r="BR51" s="17"/>
     </row>
-    <row r="52" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="55"/>
-      <c r="B52" s="61"/>
-      <c r="C52" s="61"/>
-      <c r="D52" s="61"/>
+      <c r="B52" s="59"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="59"/>
       <c r="E52" s="32"/>
       <c r="F52" s="20"/>
       <c r="G52" s="21"/>
@@ -4918,15 +4918,15 @@
       <c r="BQ52" s="22"/>
       <c r="BR52" s="20"/>
     </row>
-    <row r="53" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="55">
         <v>22</v>
       </c>
-      <c r="B53" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="C53" s="64"/>
-      <c r="D53" s="64"/>
+      <c r="B53" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" s="56"/>
+      <c r="D53" s="56"/>
       <c r="E53" s="29"/>
       <c r="F53" s="10"/>
       <c r="I53" s="12"/>
@@ -4962,11 +4962,11 @@
       <c r="BQ53" s="12"/>
       <c r="BR53" s="10"/>
     </row>
-    <row r="54" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="55"/>
-      <c r="B54" s="65"/>
-      <c r="C54" s="65"/>
-      <c r="D54" s="65"/>
+      <c r="B54" s="57"/>
+      <c r="C54" s="57"/>
+      <c r="D54" s="57"/>
       <c r="E54" s="30"/>
       <c r="F54" s="13"/>
       <c r="G54" s="14"/>
@@ -5034,15 +5034,15 @@
       <c r="BQ54" s="15"/>
       <c r="BR54" s="13"/>
     </row>
-    <row r="55" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="55">
         <v>23</v>
       </c>
-      <c r="B55" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="C55" s="60"/>
-      <c r="D55" s="60"/>
+      <c r="B55" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" s="58"/>
+      <c r="D55" s="58"/>
       <c r="E55" s="31"/>
       <c r="F55" s="17"/>
       <c r="I55" s="19"/>
@@ -5078,11 +5078,11 @@
       <c r="BQ55" s="19"/>
       <c r="BR55" s="17"/>
     </row>
-    <row r="56" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="55"/>
-      <c r="B56" s="61"/>
-      <c r="C56" s="61"/>
-      <c r="D56" s="61"/>
+      <c r="B56" s="59"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="59"/>
       <c r="E56" s="32"/>
       <c r="F56" s="20"/>
       <c r="G56" s="21"/>
@@ -5150,15 +5150,15 @@
       <c r="BQ56" s="22"/>
       <c r="BR56" s="20"/>
     </row>
-    <row r="57" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="55">
         <v>24</v>
       </c>
-      <c r="B57" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="C57" s="64"/>
-      <c r="D57" s="64"/>
+      <c r="B57" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="C57" s="56"/>
+      <c r="D57" s="56"/>
       <c r="E57" s="29"/>
       <c r="F57" s="10"/>
       <c r="I57" s="12"/>
@@ -5194,11 +5194,11 @@
       <c r="BQ57" s="12"/>
       <c r="BR57" s="10"/>
     </row>
-    <row r="58" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="55"/>
-      <c r="B58" s="65"/>
-      <c r="C58" s="65"/>
-      <c r="D58" s="65"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="57"/>
       <c r="E58" s="30"/>
       <c r="F58" s="13"/>
       <c r="G58" s="14"/>
@@ -5266,15 +5266,15 @@
       <c r="BQ58" s="15"/>
       <c r="BR58" s="13"/>
     </row>
-    <row r="59" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="55">
         <v>25</v>
       </c>
-      <c r="B59" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="C59" s="60"/>
-      <c r="D59" s="60"/>
+      <c r="B59" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C59" s="58"/>
+      <c r="D59" s="58"/>
       <c r="E59" s="31"/>
       <c r="F59" s="17"/>
       <c r="I59" s="19"/>
@@ -5310,11 +5310,11 @@
       <c r="BQ59" s="19"/>
       <c r="BR59" s="17"/>
     </row>
-    <row r="60" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="55"/>
-      <c r="B60" s="61"/>
-      <c r="C60" s="61"/>
-      <c r="D60" s="61"/>
+      <c r="B60" s="59"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="59"/>
       <c r="E60" s="32"/>
       <c r="F60" s="20"/>
       <c r="G60" s="21"/>
@@ -5382,15 +5382,15 @@
       <c r="BQ60" s="22"/>
       <c r="BR60" s="20"/>
     </row>
-    <row r="61" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="55">
         <v>26</v>
       </c>
-      <c r="B61" s="64" t="s">
-        <v>48</v>
-      </c>
-      <c r="C61" s="64"/>
-      <c r="D61" s="64"/>
+      <c r="B61" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" s="56"/>
+      <c r="D61" s="56"/>
       <c r="E61" s="29"/>
       <c r="F61" s="10"/>
       <c r="I61" s="12"/>
@@ -5426,11 +5426,11 @@
       <c r="BQ61" s="12"/>
       <c r="BR61" s="10"/>
     </row>
-    <row r="62" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="55"/>
-      <c r="B62" s="65"/>
-      <c r="C62" s="65"/>
-      <c r="D62" s="65"/>
+      <c r="B62" s="57"/>
+      <c r="C62" s="57"/>
+      <c r="D62" s="57"/>
       <c r="E62" s="30"/>
       <c r="F62" s="13"/>
       <c r="G62" s="14"/>
@@ -5498,15 +5498,15 @@
       <c r="BQ62" s="15"/>
       <c r="BR62" s="13"/>
     </row>
-    <row r="63" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:70" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="55">
         <v>27</v>
       </c>
-      <c r="B63" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="C63" s="60"/>
-      <c r="D63" s="60"/>
+      <c r="B63" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C63" s="58"/>
+      <c r="D63" s="58"/>
       <c r="E63" s="31"/>
       <c r="F63" s="17"/>
       <c r="I63" s="19"/>
@@ -5542,11 +5542,11 @@
       <c r="BQ63" s="19"/>
       <c r="BR63" s="17"/>
     </row>
-    <row r="64" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:70" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="55"/>
-      <c r="B64" s="61"/>
-      <c r="C64" s="61"/>
-      <c r="D64" s="61"/>
+      <c r="B64" s="59"/>
+      <c r="C64" s="59"/>
+      <c r="D64" s="59"/>
       <c r="E64" s="32"/>
       <c r="F64" s="20"/>
       <c r="G64" s="21"/>
@@ -5614,15 +5614,15 @@
       <c r="BQ64" s="22"/>
       <c r="BR64" s="20"/>
     </row>
-    <row r="65" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="55">
         <v>28</v>
       </c>
-      <c r="B65" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="C65" s="64"/>
-      <c r="D65" s="64"/>
+      <c r="B65" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="C65" s="56"/>
+      <c r="D65" s="56"/>
       <c r="E65" s="29"/>
       <c r="F65" s="10"/>
       <c r="I65" s="12"/>
@@ -5658,11 +5658,11 @@
       <c r="BQ65" s="12"/>
       <c r="BR65" s="10"/>
     </row>
-    <row r="66" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:70" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="55"/>
-      <c r="B66" s="65"/>
-      <c r="C66" s="65"/>
-      <c r="D66" s="65"/>
+      <c r="B66" s="57"/>
+      <c r="C66" s="57"/>
+      <c r="D66" s="57"/>
       <c r="E66" s="33"/>
       <c r="F66" s="13"/>
       <c r="G66" s="14"/>
@@ -5730,7 +5730,7 @@
       <c r="BQ66" s="15"/>
       <c r="BR66" s="13"/>
     </row>
-    <row r="67" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B67" s="6" t="s">
         <v>12</v>
       </c>
@@ -5739,6 +5739,92 @@
     </row>
   </sheetData>
   <mergeCells count="110">
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:D42"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C63:D64"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:D46"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="C65:D66"/>
+    <mergeCell ref="C51:D52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:D54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="C55:D56"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:D58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:D60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:D62"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:D26"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:D48"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:D36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:D38"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="C3:D4"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="C19:D20"/>
     <mergeCell ref="A21:A22"/>
@@ -5763,92 +5849,6 @@
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:D48"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:D34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:D36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:D38"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:D40"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:D26"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C63:D64"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:D46"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:D66"/>
-    <mergeCell ref="C51:D52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:D54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C55:D56"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:D58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:D60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:D62"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:D42"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:BQ8 F25:BQ44 F11:BQ16 F46:BQ64 F45:AV45 BC45:BQ45 AX45:BA45">
     <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">

</xml_diff>

<commit_message>
Modified Konzeptbericht and Gantt
Modified Konzeptbericht
Modified Gantt
Cleaned up docs folder
</commit_message>
<xml_diff>
--- a/doc/Projektplan Gantt.xlsx
+++ b/doc/Projektplan Gantt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="25610" windowHeight="16010"/>
+    <workbookView xWindow="0" yWindow="-435" windowWidth="25605" windowHeight="16005"/>
   </bookViews>
   <sheets>
     <sheet name="Balkenplan" sheetId="1" r:id="rId1"/>
@@ -773,32 +773,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -815,7 +794,37 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -830,23 +839,14 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="69">
@@ -1355,73 +1355,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="81" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AG29" sqref="AG29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="47.7265625" customWidth="1"/>
-    <col min="4" max="5" width="12.7265625" customWidth="1"/>
-    <col min="6" max="6" width="4.453125" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.1796875" style="5" customWidth="1"/>
-    <col min="8" max="9" width="3.1796875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="3.1796875" style="8" customWidth="1"/>
-    <col min="11" max="11" width="3.1796875" style="5" customWidth="1"/>
-    <col min="12" max="13" width="3.1796875" style="6" customWidth="1"/>
-    <col min="14" max="14" width="3.1796875" style="8" customWidth="1"/>
-    <col min="15" max="15" width="3.1796875" style="5" customWidth="1"/>
-    <col min="16" max="17" width="3.1796875" style="6" customWidth="1"/>
-    <col min="18" max="18" width="3.1796875" style="8" customWidth="1"/>
-    <col min="19" max="19" width="3.1796875" style="5" customWidth="1"/>
-    <col min="20" max="21" width="3.1796875" style="6" customWidth="1"/>
-    <col min="22" max="22" width="3.1796875" style="8" customWidth="1"/>
-    <col min="23" max="23" width="3.1796875" style="5" customWidth="1"/>
-    <col min="24" max="25" width="3.1796875" style="6" customWidth="1"/>
-    <col min="26" max="26" width="3.1796875" style="8" customWidth="1"/>
-    <col min="27" max="27" width="3.1796875" style="5" customWidth="1"/>
-    <col min="28" max="29" width="3.1796875" style="6" customWidth="1"/>
-    <col min="30" max="30" width="3.1796875" style="8" customWidth="1"/>
-    <col min="31" max="31" width="3.1796875" style="5" customWidth="1"/>
-    <col min="32" max="33" width="3.1796875" style="6" customWidth="1"/>
-    <col min="34" max="34" width="3.1796875" style="8" customWidth="1"/>
-    <col min="35" max="35" width="3.1796875" style="5" customWidth="1"/>
-    <col min="36" max="37" width="3.1796875" style="6" customWidth="1"/>
-    <col min="38" max="38" width="3.1796875" style="8" customWidth="1"/>
-    <col min="39" max="39" width="3.1796875" style="5" customWidth="1"/>
-    <col min="40" max="41" width="3.1796875" style="6" customWidth="1"/>
-    <col min="42" max="42" width="3.1796875" style="8" customWidth="1"/>
-    <col min="43" max="43" width="3.1796875" style="5" customWidth="1"/>
-    <col min="44" max="45" width="3.1796875" style="6" customWidth="1"/>
-    <col min="46" max="46" width="3.1796875" style="8" customWidth="1"/>
-    <col min="47" max="47" width="3.1796875" style="5" customWidth="1"/>
-    <col min="48" max="49" width="3.1796875" style="6" customWidth="1"/>
-    <col min="50" max="50" width="3.1796875" style="8" customWidth="1"/>
-    <col min="51" max="51" width="3.1796875" style="5" customWidth="1"/>
-    <col min="52" max="53" width="3.1796875" style="6" customWidth="1"/>
-    <col min="54" max="54" width="3.1796875" style="8" customWidth="1"/>
-    <col min="55" max="55" width="3.1796875" style="5" customWidth="1"/>
-    <col min="56" max="57" width="3.1796875" style="6" customWidth="1"/>
-    <col min="58" max="58" width="3.1796875" style="8" customWidth="1"/>
-    <col min="59" max="59" width="3.1796875" style="5" customWidth="1"/>
-    <col min="60" max="61" width="3.1796875" style="6" customWidth="1"/>
-    <col min="62" max="62" width="3.1796875" style="8" customWidth="1"/>
-    <col min="63" max="63" width="3.1796875" style="5" customWidth="1"/>
-    <col min="64" max="65" width="3.1796875" style="6" customWidth="1"/>
-    <col min="66" max="66" width="3.1796875" style="8" customWidth="1"/>
-    <col min="67" max="67" width="3.1796875" style="5" customWidth="1"/>
-    <col min="68" max="69" width="3.1796875" style="6" customWidth="1"/>
-    <col min="70" max="70" width="3.1796875" style="8" customWidth="1"/>
-    <col min="71" max="71" width="3.1796875" style="5" customWidth="1"/>
-    <col min="72" max="72" width="2.7265625" customWidth="1"/>
-    <col min="73" max="73" width="2.453125" customWidth="1"/>
-    <col min="74" max="74" width="2.1796875" customWidth="1"/>
-    <col min="75" max="75" width="2.453125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="47.7109375" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.140625" style="5" customWidth="1"/>
+    <col min="8" max="9" width="3.140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="3.140625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="3.140625" style="5" customWidth="1"/>
+    <col min="12" max="13" width="3.140625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="3.140625" style="8" customWidth="1"/>
+    <col min="15" max="15" width="3.140625" style="5" customWidth="1"/>
+    <col min="16" max="17" width="3.140625" style="6" customWidth="1"/>
+    <col min="18" max="18" width="3.140625" style="8" customWidth="1"/>
+    <col min="19" max="19" width="3.140625" style="5" customWidth="1"/>
+    <col min="20" max="21" width="3.140625" style="6" customWidth="1"/>
+    <col min="22" max="22" width="3.140625" style="8" customWidth="1"/>
+    <col min="23" max="23" width="3.140625" style="5" customWidth="1"/>
+    <col min="24" max="25" width="3.140625" style="6" customWidth="1"/>
+    <col min="26" max="26" width="3.140625" style="8" customWidth="1"/>
+    <col min="27" max="27" width="3.140625" style="5" customWidth="1"/>
+    <col min="28" max="29" width="3.140625" style="6" customWidth="1"/>
+    <col min="30" max="30" width="3.140625" style="8" customWidth="1"/>
+    <col min="31" max="31" width="3.140625" style="5" customWidth="1"/>
+    <col min="32" max="33" width="3.140625" style="6" customWidth="1"/>
+    <col min="34" max="34" width="3.140625" style="8" customWidth="1"/>
+    <col min="35" max="35" width="3.140625" style="5" customWidth="1"/>
+    <col min="36" max="37" width="3.140625" style="6" customWidth="1"/>
+    <col min="38" max="38" width="3.140625" style="8" customWidth="1"/>
+    <col min="39" max="39" width="3.140625" style="5" customWidth="1"/>
+    <col min="40" max="41" width="3.140625" style="6" customWidth="1"/>
+    <col min="42" max="42" width="3.140625" style="8" customWidth="1"/>
+    <col min="43" max="43" width="3.140625" style="5" customWidth="1"/>
+    <col min="44" max="45" width="3.140625" style="6" customWidth="1"/>
+    <col min="46" max="46" width="3.140625" style="8" customWidth="1"/>
+    <col min="47" max="47" width="3.140625" style="5" customWidth="1"/>
+    <col min="48" max="49" width="3.140625" style="6" customWidth="1"/>
+    <col min="50" max="50" width="3.140625" style="8" customWidth="1"/>
+    <col min="51" max="51" width="3.140625" style="5" customWidth="1"/>
+    <col min="52" max="53" width="3.140625" style="6" customWidth="1"/>
+    <col min="54" max="54" width="3.140625" style="8" customWidth="1"/>
+    <col min="55" max="55" width="3.140625" style="5" customWidth="1"/>
+    <col min="56" max="57" width="3.140625" style="6" customWidth="1"/>
+    <col min="58" max="58" width="3.140625" style="8" customWidth="1"/>
+    <col min="59" max="59" width="3.140625" style="5" customWidth="1"/>
+    <col min="60" max="61" width="3.140625" style="6" customWidth="1"/>
+    <col min="62" max="62" width="3.140625" style="8" customWidth="1"/>
+    <col min="63" max="63" width="3.140625" style="5" customWidth="1"/>
+    <col min="64" max="65" width="3.140625" style="6" customWidth="1"/>
+    <col min="66" max="66" width="3.140625" style="8" customWidth="1"/>
+    <col min="67" max="67" width="3.140625" style="5" customWidth="1"/>
+    <col min="68" max="69" width="3.140625" style="6" customWidth="1"/>
+    <col min="70" max="70" width="3.140625" style="8" customWidth="1"/>
+    <col min="71" max="71" width="3.140625" style="5" customWidth="1"/>
+    <col min="72" max="72" width="2.7109375" customWidth="1"/>
+    <col min="73" max="73" width="2.42578125" customWidth="1"/>
+    <col min="74" max="74" width="2.140625" customWidth="1"/>
+    <col min="75" max="75" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" s="2" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:73" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="26"/>
@@ -1431,106 +1431,106 @@
         <v>3</v>
       </c>
       <c r="F1" s="35"/>
-      <c r="G1" s="66">
+      <c r="G1" s="74">
         <v>42031</v>
       </c>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="66">
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="74">
         <v>42038</v>
       </c>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="66">
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="74">
         <v>42045</v>
       </c>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="66">
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="74">
         <v>42052</v>
       </c>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="66">
+      <c r="T1" s="75"/>
+      <c r="U1" s="75"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="74">
         <v>42059</v>
       </c>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="66">
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="76"/>
+      <c r="AA1" s="74">
         <v>42066</v>
       </c>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="66">
+      <c r="AB1" s="75"/>
+      <c r="AC1" s="75"/>
+      <c r="AD1" s="76"/>
+      <c r="AE1" s="74">
         <v>42073</v>
       </c>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="68"/>
-      <c r="AI1" s="66">
+      <c r="AF1" s="75"/>
+      <c r="AG1" s="75"/>
+      <c r="AH1" s="76"/>
+      <c r="AI1" s="74">
         <v>42080</v>
       </c>
-      <c r="AJ1" s="67"/>
-      <c r="AK1" s="67"/>
-      <c r="AL1" s="68"/>
-      <c r="AM1" s="66">
+      <c r="AJ1" s="75"/>
+      <c r="AK1" s="75"/>
+      <c r="AL1" s="76"/>
+      <c r="AM1" s="74">
         <v>42087</v>
       </c>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="68"/>
-      <c r="AQ1" s="66">
+      <c r="AN1" s="75"/>
+      <c r="AO1" s="75"/>
+      <c r="AP1" s="76"/>
+      <c r="AQ1" s="74">
         <v>42115</v>
       </c>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="68"/>
-      <c r="AU1" s="66">
+      <c r="AR1" s="75"/>
+      <c r="AS1" s="75"/>
+      <c r="AT1" s="76"/>
+      <c r="AU1" s="74">
         <v>42122</v>
       </c>
-      <c r="AV1" s="67"/>
-      <c r="AW1" s="67"/>
-      <c r="AX1" s="68"/>
-      <c r="AY1" s="66">
+      <c r="AV1" s="75"/>
+      <c r="AW1" s="75"/>
+      <c r="AX1" s="76"/>
+      <c r="AY1" s="74">
         <v>42129</v>
       </c>
-      <c r="AZ1" s="67"/>
-      <c r="BA1" s="67"/>
-      <c r="BB1" s="68"/>
-      <c r="BC1" s="66">
+      <c r="AZ1" s="75"/>
+      <c r="BA1" s="75"/>
+      <c r="BB1" s="76"/>
+      <c r="BC1" s="74">
         <v>42136</v>
       </c>
-      <c r="BD1" s="67"/>
-      <c r="BE1" s="67"/>
-      <c r="BF1" s="68"/>
-      <c r="BG1" s="66">
+      <c r="BD1" s="75"/>
+      <c r="BE1" s="75"/>
+      <c r="BF1" s="76"/>
+      <c r="BG1" s="74">
         <v>42143</v>
       </c>
-      <c r="BH1" s="67"/>
-      <c r="BI1" s="67"/>
-      <c r="BJ1" s="68"/>
-      <c r="BK1" s="66">
+      <c r="BH1" s="75"/>
+      <c r="BI1" s="75"/>
+      <c r="BJ1" s="76"/>
+      <c r="BK1" s="74">
         <v>42150</v>
       </c>
-      <c r="BL1" s="67"/>
-      <c r="BM1" s="67"/>
-      <c r="BN1" s="68"/>
-      <c r="BO1" s="66">
+      <c r="BL1" s="75"/>
+      <c r="BM1" s="75"/>
+      <c r="BN1" s="76"/>
+      <c r="BO1" s="74">
         <v>42157</v>
       </c>
-      <c r="BP1" s="67"/>
-      <c r="BQ1" s="67"/>
-      <c r="BR1" s="68"/>
+      <c r="BP1" s="75"/>
+      <c r="BQ1" s="75"/>
+      <c r="BR1" s="76"/>
       <c r="BS1" s="9"/>
     </row>
-    <row r="2" spans="1:73" s="1" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="69"/>
+    <row r="2" spans="1:73" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="89"/>
       <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
@@ -1738,18 +1738,18 @@
       <c r="BT2" s="4"/>
       <c r="BU2" s="4"/>
     </row>
-    <row r="3" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="65">
-        <v>1</v>
-      </c>
-      <c r="B3" s="84" t="s">
+    <row r="3" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="66">
+        <v>1</v>
+      </c>
+      <c r="B3" s="77" t="s">
         <v>37</v>
       </c>
       <c r="C3" s="59"/>
-      <c r="D3" s="74">
+      <c r="D3" s="67">
         <v>4</v>
       </c>
-      <c r="E3" s="74"/>
+      <c r="E3" s="67"/>
       <c r="F3" s="38" t="s">
         <v>1</v>
       </c>
@@ -1791,12 +1791,12 @@
       <c r="BR3" s="12"/>
       <c r="BS3" s="10"/>
     </row>
-    <row r="4" spans="1:73" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="65"/>
-      <c r="B4" s="85"/>
+    <row r="4" spans="1:73" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="66"/>
+      <c r="B4" s="78"/>
       <c r="C4" s="60"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
       <c r="F4" s="39" t="s">
         <v>2</v>
       </c>
@@ -1812,8 +1812,12 @@
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="15"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="14"/>
+      <c r="S4" s="13">
+        <v>2</v>
+      </c>
+      <c r="T4" s="14">
+        <v>2</v>
+      </c>
       <c r="U4" s="14"/>
       <c r="V4" s="15"/>
       <c r="W4" s="13"/>
@@ -1866,20 +1870,20 @@
       <c r="BR4" s="15"/>
       <c r="BS4" s="13"/>
     </row>
-    <row r="5" spans="1:73" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="65">
+    <row r="5" spans="1:73" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="66">
         <v>2</v>
       </c>
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="72" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="72">
+      <c r="D5" s="79">
         <v>4</v>
       </c>
-      <c r="E5" s="70"/>
+      <c r="E5" s="72"/>
       <c r="F5" s="31" t="s">
         <v>1</v>
       </c>
@@ -1922,12 +1926,12 @@
       <c r="BR5" s="19"/>
       <c r="BS5" s="17"/>
     </row>
-    <row r="6" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="65"/>
-      <c r="B6" s="71"/>
+    <row r="6" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="66"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="63"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
       <c r="F6" s="32" t="s">
         <v>2</v>
       </c>
@@ -1945,8 +1949,12 @@
       <c r="R6" s="22"/>
       <c r="S6" s="20"/>
       <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="22"/>
+      <c r="U6" s="21">
+        <v>2</v>
+      </c>
+      <c r="V6" s="22">
+        <v>2</v>
+      </c>
       <c r="W6" s="20"/>
       <c r="X6" s="21"/>
       <c r="Y6" s="21"/>
@@ -1997,20 +2005,20 @@
       <c r="BR6" s="22"/>
       <c r="BS6" s="20"/>
     </row>
-    <row r="7" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="65">
+    <row r="7" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="66">
         <v>3</v>
       </c>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="89" t="s">
+      <c r="C7" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="76">
+      <c r="D7" s="69">
         <v>4</v>
       </c>
-      <c r="E7" s="77"/>
+      <c r="E7" s="70"/>
       <c r="F7" s="29" t="s">
         <v>1</v>
       </c>
@@ -2053,12 +2061,12 @@
       <c r="BR7" s="12"/>
       <c r="BS7" s="10"/>
     </row>
-    <row r="8" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="65"/>
-      <c r="B8" s="75"/>
+    <row r="8" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="66"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="56"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="78"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="71"/>
       <c r="F8" s="30" t="s">
         <v>2</v>
       </c>
@@ -2078,9 +2086,15 @@
       <c r="T8" s="14"/>
       <c r="U8" s="14"/>
       <c r="V8" s="15"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
+      <c r="W8" s="13">
+        <v>2</v>
+      </c>
+      <c r="X8" s="14">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="14">
+        <v>2</v>
+      </c>
       <c r="Z8" s="15"/>
       <c r="AA8" s="13"/>
       <c r="AB8" s="14"/>
@@ -2128,20 +2142,20 @@
       <c r="BR8" s="15"/>
       <c r="BS8" s="13"/>
     </row>
-    <row r="9" spans="1:73" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="65">
+    <row r="9" spans="1:73" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="66">
         <v>7</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="72" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="72">
+      <c r="D9" s="79">
         <v>6</v>
       </c>
-      <c r="E9" s="70"/>
+      <c r="E9" s="72"/>
       <c r="F9" s="31" t="s">
         <v>1</v>
       </c>
@@ -2186,12 +2200,12 @@
       <c r="BR9" s="19"/>
       <c r="BS9" s="17"/>
     </row>
-    <row r="10" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="65"/>
-      <c r="B10" s="71"/>
+    <row r="10" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="66"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="58"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
       <c r="F10" s="32" t="s">
         <v>2</v>
       </c>
@@ -2214,9 +2228,15 @@
       <c r="W10" s="20"/>
       <c r="X10" s="21"/>
       <c r="Y10" s="21"/>
-      <c r="Z10" s="22"/>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="21"/>
+      <c r="Z10" s="22">
+        <v>2</v>
+      </c>
+      <c r="AA10" s="20">
+        <v>2</v>
+      </c>
+      <c r="AB10" s="21">
+        <v>2</v>
+      </c>
       <c r="AC10" s="21"/>
       <c r="AD10" s="22"/>
       <c r="AE10" s="20"/>
@@ -2261,18 +2281,18 @@
       <c r="BR10" s="22"/>
       <c r="BS10" s="20"/>
     </row>
-    <row r="11" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="65">
+    <row r="11" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="66">
         <v>4</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="89"/>
-      <c r="D11" s="76">
-        <v>1</v>
-      </c>
-      <c r="E11" s="77"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="69">
+        <v>1</v>
+      </c>
+      <c r="E11" s="70"/>
       <c r="F11" s="29" t="s">
         <v>1</v>
       </c>
@@ -2313,12 +2333,12 @@
       <c r="BR11" s="12"/>
       <c r="BS11" s="10"/>
     </row>
-    <row r="12" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="65"/>
-      <c r="B12" s="75"/>
+    <row r="12" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="66"/>
+      <c r="B12" s="68"/>
       <c r="C12" s="56"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="78"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="71"/>
       <c r="F12" s="30" t="s">
         <v>2</v>
       </c>
@@ -2344,7 +2364,9 @@
       <c r="Z12" s="15"/>
       <c r="AA12" s="13"/>
       <c r="AB12" s="14"/>
-      <c r="AC12" s="14"/>
+      <c r="AC12" s="14">
+        <v>2</v>
+      </c>
       <c r="AD12" s="15"/>
       <c r="AE12" s="13"/>
       <c r="AF12" s="14"/>
@@ -2388,20 +2410,20 @@
       <c r="BR12" s="15"/>
       <c r="BS12" s="13"/>
     </row>
-    <row r="13" spans="1:73" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="65">
+    <row r="13" spans="1:73" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="66">
         <v>5</v>
       </c>
-      <c r="B13" s="70" t="s">
+      <c r="B13" s="72" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="70">
+      <c r="D13" s="72">
         <v>4</v>
       </c>
-      <c r="E13" s="70"/>
+      <c r="E13" s="72"/>
       <c r="F13" s="31" t="s">
         <v>1</v>
       </c>
@@ -2444,12 +2466,12 @@
       <c r="BR13" s="19"/>
       <c r="BS13" s="17"/>
     </row>
-    <row r="14" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="65"/>
-      <c r="B14" s="79"/>
+    <row r="14" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="66"/>
+      <c r="B14" s="88"/>
       <c r="C14" s="64"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
       <c r="F14" s="32" t="s">
         <v>2</v>
       </c>
@@ -2476,7 +2498,9 @@
       <c r="AA14" s="20"/>
       <c r="AB14" s="21"/>
       <c r="AC14" s="21"/>
-      <c r="AD14" s="22"/>
+      <c r="AD14" s="22">
+        <v>2</v>
+      </c>
       <c r="AE14" s="20"/>
       <c r="AF14" s="21"/>
       <c r="AG14" s="21"/>
@@ -2519,20 +2543,20 @@
       <c r="BR14" s="22"/>
       <c r="BS14" s="20"/>
     </row>
-    <row r="15" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="65">
+    <row r="15" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="66">
         <v>6</v>
       </c>
-      <c r="B15" s="74" t="s">
+      <c r="B15" s="67" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="74">
+      <c r="D15" s="67">
         <v>3</v>
       </c>
-      <c r="E15" s="74"/>
+      <c r="E15" s="67"/>
       <c r="F15" s="29" t="s">
         <v>1</v>
       </c>
@@ -2575,12 +2599,12 @@
       <c r="BR15" s="12"/>
       <c r="BS15" s="10"/>
     </row>
-    <row r="16" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="65"/>
-      <c r="B16" s="75"/>
+    <row r="16" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="66"/>
+      <c r="B16" s="68"/>
       <c r="C16" s="56"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
       <c r="F16" s="30" t="s">
         <v>2</v>
       </c>
@@ -2650,18 +2674,18 @@
       <c r="BR16" s="15"/>
       <c r="BS16" s="13"/>
     </row>
-    <row r="17" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="65">
+    <row r="17" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="66">
         <v>7</v>
       </c>
-      <c r="B17" s="70" t="s">
+      <c r="B17" s="72" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="57"/>
-      <c r="D17" s="72">
+      <c r="D17" s="79">
         <v>4</v>
       </c>
-      <c r="E17" s="70"/>
+      <c r="E17" s="72"/>
       <c r="F17" s="31" t="s">
         <v>1</v>
       </c>
@@ -2704,12 +2728,12 @@
       <c r="BR17" s="19"/>
       <c r="BS17" s="17"/>
     </row>
-    <row r="18" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="65"/>
-      <c r="B18" s="71"/>
+    <row r="18" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="66"/>
+      <c r="B18" s="73"/>
       <c r="C18" s="58"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
       <c r="F18" s="32" t="s">
         <v>2</v>
       </c>
@@ -2779,8 +2803,8 @@
       <c r="BR18" s="22"/>
       <c r="BS18" s="20"/>
     </row>
-    <row r="19" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="65">
+    <row r="19" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="66">
         <v>8</v>
       </c>
       <c r="B19" s="49" t="s">
@@ -2789,10 +2813,10 @@
       <c r="C19" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="74">
+      <c r="D19" s="67">
         <v>8</v>
       </c>
-      <c r="E19" s="74"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="29" t="s">
         <v>1</v>
       </c>
@@ -2840,14 +2864,14 @@
       <c r="BR19" s="12"/>
       <c r="BS19" s="10"/>
     </row>
-    <row r="20" spans="1:71" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="65"/>
+    <row r="20" spans="1:71" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="66"/>
       <c r="B20" s="52" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="56"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="75"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
       <c r="F20" s="30" t="s">
         <v>2</v>
       </c>
@@ -2917,20 +2941,20 @@
       <c r="BR20" s="15"/>
       <c r="BS20" s="13"/>
     </row>
-    <row r="21" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="65">
+    <row r="21" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="66">
         <v>7</v>
       </c>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="72" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="72">
+      <c r="D21" s="79">
         <v>4</v>
       </c>
-      <c r="E21" s="86"/>
+      <c r="E21" s="80"/>
       <c r="F21" s="31" t="s">
         <v>1</v>
       </c>
@@ -2973,12 +2997,12 @@
       <c r="BR21" s="19"/>
       <c r="BS21" s="17"/>
     </row>
-    <row r="22" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="65"/>
-      <c r="B22" s="71"/>
+    <row r="22" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="66"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="58"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="88"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="82"/>
       <c r="F22" s="32" t="s">
         <v>2</v>
       </c>
@@ -3048,20 +3072,20 @@
       <c r="BR22" s="22"/>
       <c r="BS22" s="20"/>
     </row>
-    <row r="23" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="65">
+    <row r="23" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="66">
         <v>8</v>
       </c>
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="67" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="74">
+      <c r="D23" s="67">
         <v>4</v>
       </c>
-      <c r="E23" s="74"/>
+      <c r="E23" s="67"/>
       <c r="F23" s="29" t="s">
         <v>1</v>
       </c>
@@ -3104,12 +3128,12 @@
       <c r="BR23" s="12"/>
       <c r="BS23" s="10"/>
     </row>
-    <row r="24" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="65"/>
-      <c r="B24" s="75"/>
+    <row r="24" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="66"/>
+      <c r="B24" s="68"/>
       <c r="C24" s="56"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
       <c r="F24" s="30" t="s">
         <v>2</v>
       </c>
@@ -3179,20 +3203,20 @@
       <c r="BR24" s="15"/>
       <c r="BS24" s="13"/>
     </row>
-    <row r="25" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="65">
+    <row r="25" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="66">
         <v>7</v>
       </c>
-      <c r="B25" s="70" t="s">
+      <c r="B25" s="72" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="72">
+      <c r="D25" s="79">
         <v>4</v>
       </c>
-      <c r="E25" s="70"/>
+      <c r="E25" s="72"/>
       <c r="F25" s="31" t="s">
         <v>1</v>
       </c>
@@ -3235,12 +3259,12 @@
       <c r="BR25" s="19"/>
       <c r="BS25" s="17"/>
     </row>
-    <row r="26" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="65"/>
-      <c r="B26" s="71"/>
+    <row r="26" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="66"/>
+      <c r="B26" s="73"/>
       <c r="C26" s="58"/>
-      <c r="D26" s="71"/>
-      <c r="E26" s="71"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
       <c r="F26" s="32" t="s">
         <v>2</v>
       </c>
@@ -3310,20 +3334,20 @@
       <c r="BR26" s="22"/>
       <c r="BS26" s="20"/>
     </row>
-    <row r="27" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="65">
+    <row r="27" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="66">
         <v>8</v>
       </c>
-      <c r="B27" s="74" t="s">
+      <c r="B27" s="67" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="74">
+      <c r="D27" s="67">
         <v>4</v>
       </c>
-      <c r="E27" s="74"/>
+      <c r="E27" s="67"/>
       <c r="F27" s="29" t="s">
         <v>1</v>
       </c>
@@ -3366,12 +3390,12 @@
       <c r="BR27" s="12"/>
       <c r="BS27" s="10"/>
     </row>
-    <row r="28" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="65"/>
-      <c r="B28" s="75"/>
+    <row r="28" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="66"/>
+      <c r="B28" s="68"/>
       <c r="C28" s="56"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
       <c r="F28" s="30" t="s">
         <v>2</v>
       </c>
@@ -3441,20 +3465,20 @@
       <c r="BR28" s="15"/>
       <c r="BS28" s="13"/>
     </row>
-    <row r="29" spans="1:71" s="18" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="65">
+    <row r="29" spans="1:71" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="66">
         <v>9</v>
       </c>
-      <c r="B29" s="70" t="s">
+      <c r="B29" s="72" t="s">
         <v>51</v>
       </c>
       <c r="C29" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="70">
+      <c r="D29" s="72">
         <v>12</v>
       </c>
-      <c r="E29" s="70"/>
+      <c r="E29" s="72"/>
       <c r="F29" s="31" t="s">
         <v>1</v>
       </c>
@@ -3522,12 +3546,12 @@
       <c r="BR29" s="19"/>
       <c r="BS29" s="17"/>
     </row>
-    <row r="30" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="65"/>
-      <c r="B30" s="71"/>
+    <row r="30" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="66"/>
+      <c r="B30" s="73"/>
       <c r="C30" s="58"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="73"/>
       <c r="F30" s="32" t="s">
         <v>2</v>
       </c>
@@ -3597,18 +3621,18 @@
       <c r="BR30" s="22"/>
       <c r="BS30" s="20"/>
     </row>
-    <row r="31" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="65">
+    <row r="31" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="66">
         <v>10</v>
       </c>
-      <c r="B31" s="74" t="s">
+      <c r="B31" s="67" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="55"/>
-      <c r="D31" s="74">
+      <c r="D31" s="67">
         <v>8</v>
       </c>
-      <c r="E31" s="74"/>
+      <c r="E31" s="67"/>
       <c r="F31" s="29" t="s">
         <v>1</v>
       </c>
@@ -3656,12 +3680,12 @@
       <c r="BR31" s="12"/>
       <c r="BS31" s="10"/>
     </row>
-    <row r="32" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="65"/>
-      <c r="B32" s="75"/>
+    <row r="32" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="66"/>
+      <c r="B32" s="68"/>
       <c r="C32" s="56"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
       <c r="F32" s="30" t="s">
         <v>2</v>
       </c>
@@ -3731,18 +3755,18 @@
       <c r="BR32" s="15"/>
       <c r="BS32" s="13"/>
     </row>
-    <row r="33" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="65">
+    <row r="33" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="66">
         <v>11</v>
       </c>
-      <c r="B33" s="70" t="s">
+      <c r="B33" s="72" t="s">
         <v>24</v>
       </c>
       <c r="C33" s="57"/>
-      <c r="D33" s="70">
+      <c r="D33" s="72">
         <v>8</v>
       </c>
-      <c r="E33" s="70"/>
+      <c r="E33" s="72"/>
       <c r="F33" s="31" t="s">
         <v>1</v>
       </c>
@@ -3830,12 +3854,12 @@
       <c r="BR33" s="19"/>
       <c r="BS33" s="17"/>
     </row>
-    <row r="34" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="65"/>
-      <c r="B34" s="71"/>
+    <row r="34" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="66"/>
+      <c r="B34" s="73"/>
       <c r="C34" s="58"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
       <c r="F34" s="32" t="s">
         <v>2</v>
       </c>
@@ -3905,18 +3929,18 @@
       <c r="BR34" s="22"/>
       <c r="BS34" s="20"/>
     </row>
-    <row r="35" spans="1:71" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="65">
+    <row r="35" spans="1:71" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="66">
         <v>12</v>
       </c>
-      <c r="B35" s="84" t="s">
+      <c r="B35" s="77" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="59"/>
-      <c r="D35" s="74">
+      <c r="D35" s="67">
         <v>2</v>
       </c>
-      <c r="E35" s="74"/>
+      <c r="E35" s="67"/>
       <c r="F35" s="29" t="s">
         <v>1</v>
       </c>
@@ -3956,12 +3980,12 @@
       <c r="BR35" s="12"/>
       <c r="BS35" s="10"/>
     </row>
-    <row r="36" spans="1:71" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="65"/>
-      <c r="B36" s="85"/>
+    <row r="36" spans="1:71" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="66"/>
+      <c r="B36" s="78"/>
       <c r="C36" s="60"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="68"/>
       <c r="F36" s="30" t="s">
         <v>2</v>
       </c>
@@ -4031,18 +4055,18 @@
       <c r="BR36" s="15"/>
       <c r="BS36" s="13"/>
     </row>
-    <row r="37" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="65">
+    <row r="37" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="66">
         <v>13</v>
       </c>
-      <c r="B37" s="70" t="s">
+      <c r="B37" s="72" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="57"/>
-      <c r="D37" s="70">
+      <c r="D37" s="72">
         <v>6</v>
       </c>
-      <c r="E37" s="70"/>
+      <c r="E37" s="72"/>
       <c r="F37" s="31" t="s">
         <v>1</v>
       </c>
@@ -4093,12 +4117,12 @@
       <c r="BR37" s="19"/>
       <c r="BS37" s="17"/>
     </row>
-    <row r="38" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="65"/>
-      <c r="B38" s="71"/>
+    <row r="38" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="66"/>
+      <c r="B38" s="73"/>
       <c r="C38" s="58"/>
-      <c r="D38" s="71"/>
-      <c r="E38" s="71"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
       <c r="F38" s="32" t="s">
         <v>2</v>
       </c>
@@ -4168,18 +4192,18 @@
       <c r="BR38" s="22"/>
       <c r="BS38" s="20"/>
     </row>
-    <row r="39" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="65">
+    <row r="39" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="66">
         <v>14</v>
       </c>
-      <c r="B39" s="74" t="s">
+      <c r="B39" s="67" t="s">
         <v>39</v>
       </c>
       <c r="C39" s="55"/>
-      <c r="D39" s="74">
+      <c r="D39" s="67">
         <v>4</v>
       </c>
-      <c r="E39" s="74"/>
+      <c r="E39" s="67"/>
       <c r="F39" s="29" t="s">
         <v>1</v>
       </c>
@@ -4227,12 +4251,12 @@
       <c r="BR39" s="12"/>
       <c r="BS39" s="10"/>
     </row>
-    <row r="40" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="65"/>
-      <c r="B40" s="75"/>
+    <row r="40" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="66"/>
+      <c r="B40" s="68"/>
       <c r="C40" s="56"/>
-      <c r="D40" s="75"/>
-      <c r="E40" s="75"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
       <c r="F40" s="30" t="s">
         <v>2</v>
       </c>
@@ -4302,14 +4326,14 @@
       <c r="BR40" s="15"/>
       <c r="BS40" s="13"/>
     </row>
-    <row r="41" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="65">
+    <row r="41" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="66">
         <v>15</v>
       </c>
-      <c r="B41" s="70"/>
+      <c r="B41" s="72"/>
       <c r="C41" s="57"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
+      <c r="D41" s="72"/>
+      <c r="E41" s="72"/>
       <c r="F41" s="31" t="s">
         <v>1</v>
       </c>
@@ -4347,12 +4371,12 @@
       <c r="BR41" s="19"/>
       <c r="BS41" s="17"/>
     </row>
-    <row r="42" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="65"/>
-      <c r="B42" s="71"/>
+    <row r="42" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="66"/>
+      <c r="B42" s="73"/>
       <c r="C42" s="58"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="73"/>
       <c r="F42" s="32" t="s">
         <v>2</v>
       </c>
@@ -4422,8 +4446,8 @@
       <c r="BR42" s="22"/>
       <c r="BS42" s="20"/>
     </row>
-    <row r="43" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="65">
+    <row r="43" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="66">
         <v>16</v>
       </c>
       <c r="B43" s="49"/>
@@ -4467,8 +4491,8 @@
       <c r="BR43" s="12"/>
       <c r="BS43" s="10"/>
     </row>
-    <row r="44" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="65"/>
+    <row r="44" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="66"/>
       <c r="B44" s="50"/>
       <c r="C44" s="60"/>
       <c r="D44" s="52"/>
@@ -4542,16 +4566,16 @@
       <c r="BR44" s="15"/>
       <c r="BS44" s="13"/>
     </row>
-    <row r="45" spans="1:71" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A45" s="65">
+    <row r="45" spans="1:71" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A45" s="66">
         <v>18</v>
       </c>
-      <c r="B45" s="80" t="s">
+      <c r="B45" s="83" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="61"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="82"/>
+      <c r="D45" s="85"/>
+      <c r="E45" s="85"/>
       <c r="F45" s="40"/>
       <c r="G45" s="41"/>
       <c r="H45" s="42"/>
@@ -4639,12 +4663,12 @@
       <c r="BR45" s="43"/>
       <c r="BS45" s="10"/>
     </row>
-    <row r="46" spans="1:71" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A46" s="65"/>
-      <c r="B46" s="81"/>
+    <row r="46" spans="1:71" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A46" s="66"/>
+      <c r="B46" s="84"/>
       <c r="C46" s="62"/>
-      <c r="D46" s="83"/>
-      <c r="E46" s="83"/>
+      <c r="D46" s="86"/>
+      <c r="E46" s="86"/>
       <c r="F46" s="44"/>
       <c r="G46" s="45"/>
       <c r="H46" s="46"/>
@@ -4712,16 +4736,16 @@
       <c r="BR46" s="47"/>
       <c r="BS46" s="13"/>
     </row>
-    <row r="47" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="65">
+    <row r="47" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="66">
         <v>19</v>
       </c>
-      <c r="B47" s="70" t="s">
+      <c r="B47" s="72" t="s">
         <v>40</v>
       </c>
       <c r="C47" s="57"/>
-      <c r="D47" s="70"/>
-      <c r="E47" s="70"/>
+      <c r="D47" s="72"/>
+      <c r="E47" s="72"/>
       <c r="F47" s="31"/>
       <c r="G47" s="17"/>
       <c r="J47" s="19"/>
@@ -4757,12 +4781,12 @@
       <c r="BR47" s="19"/>
       <c r="BS47" s="17"/>
     </row>
-    <row r="48" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="65"/>
-      <c r="B48" s="71"/>
+    <row r="48" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="66"/>
+      <c r="B48" s="73"/>
       <c r="C48" s="58"/>
-      <c r="D48" s="71"/>
-      <c r="E48" s="71"/>
+      <c r="D48" s="73"/>
+      <c r="E48" s="73"/>
       <c r="F48" s="32"/>
       <c r="G48" s="20"/>
       <c r="H48" s="21"/>
@@ -4830,16 +4854,16 @@
       <c r="BR48" s="22"/>
       <c r="BS48" s="20"/>
     </row>
-    <row r="49" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="65">
+    <row r="49" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="66">
         <v>20</v>
       </c>
-      <c r="B49" s="74" t="s">
+      <c r="B49" s="67" t="s">
         <v>41</v>
       </c>
       <c r="C49" s="55"/>
-      <c r="D49" s="74"/>
-      <c r="E49" s="74"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="67"/>
       <c r="F49" s="29"/>
       <c r="G49" s="10"/>
       <c r="J49" s="12"/>
@@ -4875,12 +4899,12 @@
       <c r="BR49" s="12"/>
       <c r="BS49" s="10"/>
     </row>
-    <row r="50" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="65"/>
-      <c r="B50" s="75"/>
+    <row r="50" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="66"/>
+      <c r="B50" s="68"/>
       <c r="C50" s="56"/>
-      <c r="D50" s="75"/>
-      <c r="E50" s="75"/>
+      <c r="D50" s="68"/>
+      <c r="E50" s="68"/>
       <c r="F50" s="30"/>
       <c r="G50" s="13"/>
       <c r="H50" s="14"/>
@@ -4948,16 +4972,16 @@
       <c r="BR50" s="15"/>
       <c r="BS50" s="13"/>
     </row>
-    <row r="51" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="65">
+    <row r="51" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="66">
         <v>21</v>
       </c>
-      <c r="B51" s="70" t="s">
+      <c r="B51" s="72" t="s">
         <v>42</v>
       </c>
       <c r="C51" s="57"/>
-      <c r="D51" s="70"/>
-      <c r="E51" s="70"/>
+      <c r="D51" s="72"/>
+      <c r="E51" s="72"/>
       <c r="F51" s="31"/>
       <c r="G51" s="17"/>
       <c r="J51" s="19"/>
@@ -4993,12 +5017,12 @@
       <c r="BR51" s="19"/>
       <c r="BS51" s="17"/>
     </row>
-    <row r="52" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="65"/>
-      <c r="B52" s="71"/>
+    <row r="52" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="66"/>
+      <c r="B52" s="73"/>
       <c r="C52" s="58"/>
-      <c r="D52" s="71"/>
-      <c r="E52" s="71"/>
+      <c r="D52" s="73"/>
+      <c r="E52" s="73"/>
       <c r="F52" s="32"/>
       <c r="G52" s="20"/>
       <c r="H52" s="21"/>
@@ -5066,16 +5090,16 @@
       <c r="BR52" s="22"/>
       <c r="BS52" s="20"/>
     </row>
-    <row r="53" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="65">
+    <row r="53" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="66">
         <v>22</v>
       </c>
-      <c r="B53" s="74" t="s">
+      <c r="B53" s="67" t="s">
         <v>43</v>
       </c>
       <c r="C53" s="55"/>
-      <c r="D53" s="74"/>
-      <c r="E53" s="74"/>
+      <c r="D53" s="67"/>
+      <c r="E53" s="67"/>
       <c r="F53" s="29"/>
       <c r="G53" s="10"/>
       <c r="J53" s="12"/>
@@ -5111,12 +5135,12 @@
       <c r="BR53" s="12"/>
       <c r="BS53" s="10"/>
     </row>
-    <row r="54" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="65"/>
-      <c r="B54" s="75"/>
+    <row r="54" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="66"/>
+      <c r="B54" s="68"/>
       <c r="C54" s="56"/>
-      <c r="D54" s="75"/>
-      <c r="E54" s="75"/>
+      <c r="D54" s="68"/>
+      <c r="E54" s="68"/>
       <c r="F54" s="30"/>
       <c r="G54" s="13"/>
       <c r="H54" s="14"/>
@@ -5184,16 +5208,16 @@
       <c r="BR54" s="15"/>
       <c r="BS54" s="13"/>
     </row>
-    <row r="55" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="65">
+    <row r="55" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="66">
         <v>23</v>
       </c>
-      <c r="B55" s="70" t="s">
+      <c r="B55" s="72" t="s">
         <v>44</v>
       </c>
       <c r="C55" s="57"/>
-      <c r="D55" s="70"/>
-      <c r="E55" s="70"/>
+      <c r="D55" s="72"/>
+      <c r="E55" s="72"/>
       <c r="F55" s="31"/>
       <c r="G55" s="17"/>
       <c r="J55" s="19"/>
@@ -5229,12 +5253,12 @@
       <c r="BR55" s="19"/>
       <c r="BS55" s="17"/>
     </row>
-    <row r="56" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="65"/>
-      <c r="B56" s="71"/>
+    <row r="56" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="66"/>
+      <c r="B56" s="73"/>
       <c r="C56" s="58"/>
-      <c r="D56" s="71"/>
-      <c r="E56" s="71"/>
+      <c r="D56" s="73"/>
+      <c r="E56" s="73"/>
       <c r="F56" s="32"/>
       <c r="G56" s="20"/>
       <c r="H56" s="21"/>
@@ -5302,16 +5326,16 @@
       <c r="BR56" s="22"/>
       <c r="BS56" s="20"/>
     </row>
-    <row r="57" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="65">
+    <row r="57" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="66">
         <v>24</v>
       </c>
-      <c r="B57" s="74" t="s">
+      <c r="B57" s="67" t="s">
         <v>45</v>
       </c>
       <c r="C57" s="55"/>
-      <c r="D57" s="74"/>
-      <c r="E57" s="74"/>
+      <c r="D57" s="67"/>
+      <c r="E57" s="67"/>
       <c r="F57" s="29"/>
       <c r="G57" s="10"/>
       <c r="J57" s="12"/>
@@ -5347,12 +5371,12 @@
       <c r="BR57" s="12"/>
       <c r="BS57" s="10"/>
     </row>
-    <row r="58" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="65"/>
-      <c r="B58" s="75"/>
+    <row r="58" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="66"/>
+      <c r="B58" s="68"/>
       <c r="C58" s="56"/>
-      <c r="D58" s="75"/>
-      <c r="E58" s="75"/>
+      <c r="D58" s="68"/>
+      <c r="E58" s="68"/>
       <c r="F58" s="30"/>
       <c r="G58" s="13"/>
       <c r="H58" s="14"/>
@@ -5420,16 +5444,16 @@
       <c r="BR58" s="15"/>
       <c r="BS58" s="13"/>
     </row>
-    <row r="59" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="65">
+    <row r="59" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="66">
         <v>25</v>
       </c>
-      <c r="B59" s="70" t="s">
+      <c r="B59" s="72" t="s">
         <v>46</v>
       </c>
       <c r="C59" s="57"/>
-      <c r="D59" s="70"/>
-      <c r="E59" s="70"/>
+      <c r="D59" s="72"/>
+      <c r="E59" s="72"/>
       <c r="F59" s="31"/>
       <c r="G59" s="17"/>
       <c r="J59" s="19"/>
@@ -5465,12 +5489,12 @@
       <c r="BR59" s="19"/>
       <c r="BS59" s="17"/>
     </row>
-    <row r="60" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="65"/>
-      <c r="B60" s="71"/>
+    <row r="60" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="66"/>
+      <c r="B60" s="73"/>
       <c r="C60" s="58"/>
-      <c r="D60" s="71"/>
-      <c r="E60" s="71"/>
+      <c r="D60" s="73"/>
+      <c r="E60" s="73"/>
       <c r="F60" s="32"/>
       <c r="G60" s="20"/>
       <c r="H60" s="21"/>
@@ -5538,16 +5562,16 @@
       <c r="BR60" s="22"/>
       <c r="BS60" s="20"/>
     </row>
-    <row r="61" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="65">
+    <row r="61" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="66">
         <v>26</v>
       </c>
-      <c r="B61" s="74" t="s">
+      <c r="B61" s="67" t="s">
         <v>47</v>
       </c>
       <c r="C61" s="55"/>
-      <c r="D61" s="74"/>
-      <c r="E61" s="74"/>
+      <c r="D61" s="67"/>
+      <c r="E61" s="67"/>
       <c r="F61" s="29"/>
       <c r="G61" s="10"/>
       <c r="J61" s="12"/>
@@ -5583,12 +5607,12 @@
       <c r="BR61" s="12"/>
       <c r="BS61" s="10"/>
     </row>
-    <row r="62" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="65"/>
-      <c r="B62" s="75"/>
+    <row r="62" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="66"/>
+      <c r="B62" s="68"/>
       <c r="C62" s="56"/>
-      <c r="D62" s="75"/>
-      <c r="E62" s="75"/>
+      <c r="D62" s="68"/>
+      <c r="E62" s="68"/>
       <c r="F62" s="30"/>
       <c r="G62" s="13"/>
       <c r="H62" s="14"/>
@@ -5656,16 +5680,16 @@
       <c r="BR62" s="15"/>
       <c r="BS62" s="13"/>
     </row>
-    <row r="63" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="65">
+    <row r="63" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="66">
         <v>27</v>
       </c>
-      <c r="B63" s="70" t="s">
+      <c r="B63" s="72" t="s">
         <v>48</v>
       </c>
       <c r="C63" s="57"/>
-      <c r="D63" s="70"/>
-      <c r="E63" s="70"/>
+      <c r="D63" s="72"/>
+      <c r="E63" s="72"/>
       <c r="F63" s="31"/>
       <c r="G63" s="17"/>
       <c r="J63" s="19"/>
@@ -5701,12 +5725,12 @@
       <c r="BR63" s="19"/>
       <c r="BS63" s="17"/>
     </row>
-    <row r="64" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="65"/>
-      <c r="B64" s="71"/>
+    <row r="64" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="66"/>
+      <c r="B64" s="73"/>
       <c r="C64" s="58"/>
-      <c r="D64" s="71"/>
-      <c r="E64" s="71"/>
+      <c r="D64" s="73"/>
+      <c r="E64" s="73"/>
       <c r="F64" s="32"/>
       <c r="G64" s="20"/>
       <c r="H64" s="21"/>
@@ -5774,16 +5798,16 @@
       <c r="BR64" s="22"/>
       <c r="BS64" s="20"/>
     </row>
-    <row r="65" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="65">
+    <row r="65" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="66">
         <v>28</v>
       </c>
-      <c r="B65" s="74" t="s">
+      <c r="B65" s="67" t="s">
         <v>49</v>
       </c>
       <c r="C65" s="55"/>
-      <c r="D65" s="74"/>
-      <c r="E65" s="74"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="67"/>
       <c r="F65" s="29"/>
       <c r="G65" s="10"/>
       <c r="J65" s="12"/>
@@ -5819,12 +5843,12 @@
       <c r="BR65" s="12"/>
       <c r="BS65" s="10"/>
     </row>
-    <row r="66" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="65"/>
-      <c r="B66" s="75"/>
+    <row r="66" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="66"/>
+      <c r="B66" s="68"/>
       <c r="C66" s="56"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="68"/>
       <c r="F66" s="33"/>
       <c r="G66" s="13"/>
       <c r="H66" s="14"/>
@@ -5892,7 +5916,7 @@
       <c r="BR66" s="15"/>
       <c r="BS66" s="13"/>
     </row>
-    <row r="67" spans="1:71" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B67" s="6" t="s">
         <v>12</v>
       </c>
@@ -5902,25 +5926,72 @@
     </row>
   </sheetData>
   <mergeCells count="110">
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:E50"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:E8"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="D27:E28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D29:E30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="D31:E32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="AQ1:AT1"/>
+    <mergeCell ref="AU1:AX1"/>
+    <mergeCell ref="AY1:BB1"/>
+    <mergeCell ref="BO1:BR1"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AM1:AP1"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="AA1:AD1"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="D63:E64"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D45:E46"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="D65:E66"/>
+    <mergeCell ref="D51:E52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:E54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="D55:E56"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="D57:E58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="D59:E60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="D61:E62"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:E24"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:E10"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="D41:E42"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D25:E26"/>
     <mergeCell ref="BC1:BF1"/>
     <mergeCell ref="BG1:BJ1"/>
     <mergeCell ref="BK1:BN1"/>
@@ -5945,73 +6016,26 @@
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="D21:E22"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:E24"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:E10"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="D63:E64"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D45:E46"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="D65:E66"/>
-    <mergeCell ref="D51:E52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:E54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="D55:E56"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="D57:E58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="D59:E60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="D61:E62"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="D41:E42"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:E6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:E12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D13:E14"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D25:E26"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:E50"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D27:E28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D29:E30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="D31:E32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A45:A46"/>
     <mergeCell ref="D17:E18"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="AQ1:AT1"/>
-    <mergeCell ref="AU1:AX1"/>
-    <mergeCell ref="AY1:BB1"/>
-    <mergeCell ref="BO1:BR1"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AM1:AP1"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="AA1:AD1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:BR8 G25:BR44 G11:BR16 G46:BR64 G45:AW45 BD45:BR45 AY45:BB45">
     <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">

</xml_diff>

<commit_message>
modified gantt, fixed typos in elemente excel
</commit_message>
<xml_diff>
--- a/doc/Projektplan Gantt.xlsx
+++ b/doc/Projektplan Gantt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-435" windowWidth="25605" windowHeight="16005"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="25610" windowHeight="16010"/>
   </bookViews>
   <sheets>
     <sheet name="Balkenplan" sheetId="1" r:id="rId1"/>
@@ -779,27 +779,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -809,22 +788,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -839,14 +809,44 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="69">
@@ -1355,73 +1355,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AG29" sqref="AG29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AG16" sqref="AG16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="47.7109375" customWidth="1"/>
-    <col min="4" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.140625" style="5" customWidth="1"/>
-    <col min="8" max="9" width="3.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="3.140625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="3.140625" style="5" customWidth="1"/>
-    <col min="12" max="13" width="3.140625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="3.140625" style="8" customWidth="1"/>
-    <col min="15" max="15" width="3.140625" style="5" customWidth="1"/>
-    <col min="16" max="17" width="3.140625" style="6" customWidth="1"/>
-    <col min="18" max="18" width="3.140625" style="8" customWidth="1"/>
-    <col min="19" max="19" width="3.140625" style="5" customWidth="1"/>
-    <col min="20" max="21" width="3.140625" style="6" customWidth="1"/>
-    <col min="22" max="22" width="3.140625" style="8" customWidth="1"/>
-    <col min="23" max="23" width="3.140625" style="5" customWidth="1"/>
-    <col min="24" max="25" width="3.140625" style="6" customWidth="1"/>
-    <col min="26" max="26" width="3.140625" style="8" customWidth="1"/>
-    <col min="27" max="27" width="3.140625" style="5" customWidth="1"/>
-    <col min="28" max="29" width="3.140625" style="6" customWidth="1"/>
-    <col min="30" max="30" width="3.140625" style="8" customWidth="1"/>
-    <col min="31" max="31" width="3.140625" style="5" customWidth="1"/>
-    <col min="32" max="33" width="3.140625" style="6" customWidth="1"/>
-    <col min="34" max="34" width="3.140625" style="8" customWidth="1"/>
-    <col min="35" max="35" width="3.140625" style="5" customWidth="1"/>
-    <col min="36" max="37" width="3.140625" style="6" customWidth="1"/>
-    <col min="38" max="38" width="3.140625" style="8" customWidth="1"/>
-    <col min="39" max="39" width="3.140625" style="5" customWidth="1"/>
-    <col min="40" max="41" width="3.140625" style="6" customWidth="1"/>
-    <col min="42" max="42" width="3.140625" style="8" customWidth="1"/>
-    <col min="43" max="43" width="3.140625" style="5" customWidth="1"/>
-    <col min="44" max="45" width="3.140625" style="6" customWidth="1"/>
-    <col min="46" max="46" width="3.140625" style="8" customWidth="1"/>
-    <col min="47" max="47" width="3.140625" style="5" customWidth="1"/>
-    <col min="48" max="49" width="3.140625" style="6" customWidth="1"/>
-    <col min="50" max="50" width="3.140625" style="8" customWidth="1"/>
-    <col min="51" max="51" width="3.140625" style="5" customWidth="1"/>
-    <col min="52" max="53" width="3.140625" style="6" customWidth="1"/>
-    <col min="54" max="54" width="3.140625" style="8" customWidth="1"/>
-    <col min="55" max="55" width="3.140625" style="5" customWidth="1"/>
-    <col min="56" max="57" width="3.140625" style="6" customWidth="1"/>
-    <col min="58" max="58" width="3.140625" style="8" customWidth="1"/>
-    <col min="59" max="59" width="3.140625" style="5" customWidth="1"/>
-    <col min="60" max="61" width="3.140625" style="6" customWidth="1"/>
-    <col min="62" max="62" width="3.140625" style="8" customWidth="1"/>
-    <col min="63" max="63" width="3.140625" style="5" customWidth="1"/>
-    <col min="64" max="65" width="3.140625" style="6" customWidth="1"/>
-    <col min="66" max="66" width="3.140625" style="8" customWidth="1"/>
-    <col min="67" max="67" width="3.140625" style="5" customWidth="1"/>
-    <col min="68" max="69" width="3.140625" style="6" customWidth="1"/>
-    <col min="70" max="70" width="3.140625" style="8" customWidth="1"/>
-    <col min="71" max="71" width="3.140625" style="5" customWidth="1"/>
-    <col min="72" max="72" width="2.7109375" customWidth="1"/>
-    <col min="73" max="73" width="2.42578125" customWidth="1"/>
-    <col min="74" max="74" width="2.140625" customWidth="1"/>
-    <col min="75" max="75" width="2.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="47.7265625" customWidth="1"/>
+    <col min="4" max="5" width="12.7265625" customWidth="1"/>
+    <col min="6" max="6" width="4.453125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.1796875" style="5" customWidth="1"/>
+    <col min="8" max="9" width="3.1796875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="3.1796875" style="8" customWidth="1"/>
+    <col min="11" max="11" width="3.1796875" style="5" customWidth="1"/>
+    <col min="12" max="13" width="3.1796875" style="6" customWidth="1"/>
+    <col min="14" max="14" width="3.1796875" style="8" customWidth="1"/>
+    <col min="15" max="15" width="3.1796875" style="5" customWidth="1"/>
+    <col min="16" max="17" width="3.1796875" style="6" customWidth="1"/>
+    <col min="18" max="18" width="3.1796875" style="8" customWidth="1"/>
+    <col min="19" max="19" width="3.1796875" style="5" customWidth="1"/>
+    <col min="20" max="21" width="3.1796875" style="6" customWidth="1"/>
+    <col min="22" max="22" width="3.1796875" style="8" customWidth="1"/>
+    <col min="23" max="23" width="3.1796875" style="5" customWidth="1"/>
+    <col min="24" max="25" width="3.1796875" style="6" customWidth="1"/>
+    <col min="26" max="26" width="3.1796875" style="8" customWidth="1"/>
+    <col min="27" max="27" width="3.1796875" style="5" customWidth="1"/>
+    <col min="28" max="29" width="3.1796875" style="6" customWidth="1"/>
+    <col min="30" max="30" width="3.1796875" style="8" customWidth="1"/>
+    <col min="31" max="31" width="3.1796875" style="5" customWidth="1"/>
+    <col min="32" max="33" width="3.1796875" style="6" customWidth="1"/>
+    <col min="34" max="34" width="3.1796875" style="8" customWidth="1"/>
+    <col min="35" max="35" width="3.1796875" style="5" customWidth="1"/>
+    <col min="36" max="37" width="3.1796875" style="6" customWidth="1"/>
+    <col min="38" max="38" width="3.1796875" style="8" customWidth="1"/>
+    <col min="39" max="39" width="3.1796875" style="5" customWidth="1"/>
+    <col min="40" max="41" width="3.1796875" style="6" customWidth="1"/>
+    <col min="42" max="42" width="3.1796875" style="8" customWidth="1"/>
+    <col min="43" max="43" width="3.1796875" style="5" customWidth="1"/>
+    <col min="44" max="45" width="3.1796875" style="6" customWidth="1"/>
+    <col min="46" max="46" width="3.1796875" style="8" customWidth="1"/>
+    <col min="47" max="47" width="3.1796875" style="5" customWidth="1"/>
+    <col min="48" max="49" width="3.1796875" style="6" customWidth="1"/>
+    <col min="50" max="50" width="3.1796875" style="8" customWidth="1"/>
+    <col min="51" max="51" width="3.1796875" style="5" customWidth="1"/>
+    <col min="52" max="53" width="3.1796875" style="6" customWidth="1"/>
+    <col min="54" max="54" width="3.1796875" style="8" customWidth="1"/>
+    <col min="55" max="55" width="3.1796875" style="5" customWidth="1"/>
+    <col min="56" max="57" width="3.1796875" style="6" customWidth="1"/>
+    <col min="58" max="58" width="3.1796875" style="8" customWidth="1"/>
+    <col min="59" max="59" width="3.1796875" style="5" customWidth="1"/>
+    <col min="60" max="61" width="3.1796875" style="6" customWidth="1"/>
+    <col min="62" max="62" width="3.1796875" style="8" customWidth="1"/>
+    <col min="63" max="63" width="3.1796875" style="5" customWidth="1"/>
+    <col min="64" max="65" width="3.1796875" style="6" customWidth="1"/>
+    <col min="66" max="66" width="3.1796875" style="8" customWidth="1"/>
+    <col min="67" max="67" width="3.1796875" style="5" customWidth="1"/>
+    <col min="68" max="69" width="3.1796875" style="6" customWidth="1"/>
+    <col min="70" max="70" width="3.1796875" style="8" customWidth="1"/>
+    <col min="71" max="71" width="3.1796875" style="5" customWidth="1"/>
+    <col min="72" max="72" width="2.7265625" customWidth="1"/>
+    <col min="73" max="73" width="2.453125" customWidth="1"/>
+    <col min="74" max="74" width="2.1796875" customWidth="1"/>
+    <col min="75" max="75" width="2.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:73" s="2" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="26"/>
@@ -1431,106 +1431,106 @@
         <v>3</v>
       </c>
       <c r="F1" s="35"/>
-      <c r="G1" s="74">
+      <c r="G1" s="67">
         <v>42031</v>
       </c>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="74">
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="67">
         <v>42038</v>
       </c>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="74">
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="67">
         <v>42045</v>
       </c>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="74">
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="67">
         <v>42052</v>
       </c>
-      <c r="T1" s="75"/>
-      <c r="U1" s="75"/>
-      <c r="V1" s="76"/>
-      <c r="W1" s="74">
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="67">
         <v>42059</v>
       </c>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="76"/>
-      <c r="AA1" s="74">
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="69"/>
+      <c r="AA1" s="67">
         <v>42066</v>
       </c>
-      <c r="AB1" s="75"/>
-      <c r="AC1" s="75"/>
-      <c r="AD1" s="76"/>
-      <c r="AE1" s="74">
+      <c r="AB1" s="68"/>
+      <c r="AC1" s="68"/>
+      <c r="AD1" s="69"/>
+      <c r="AE1" s="67">
         <v>42073</v>
       </c>
-      <c r="AF1" s="75"/>
-      <c r="AG1" s="75"/>
-      <c r="AH1" s="76"/>
-      <c r="AI1" s="74">
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="68"/>
+      <c r="AH1" s="69"/>
+      <c r="AI1" s="67">
         <v>42080</v>
       </c>
-      <c r="AJ1" s="75"/>
-      <c r="AK1" s="75"/>
-      <c r="AL1" s="76"/>
-      <c r="AM1" s="74">
+      <c r="AJ1" s="68"/>
+      <c r="AK1" s="68"/>
+      <c r="AL1" s="69"/>
+      <c r="AM1" s="67">
         <v>42087</v>
       </c>
-      <c r="AN1" s="75"/>
-      <c r="AO1" s="75"/>
-      <c r="AP1" s="76"/>
-      <c r="AQ1" s="74">
+      <c r="AN1" s="68"/>
+      <c r="AO1" s="68"/>
+      <c r="AP1" s="69"/>
+      <c r="AQ1" s="67">
         <v>42115</v>
       </c>
-      <c r="AR1" s="75"/>
-      <c r="AS1" s="75"/>
-      <c r="AT1" s="76"/>
-      <c r="AU1" s="74">
+      <c r="AR1" s="68"/>
+      <c r="AS1" s="68"/>
+      <c r="AT1" s="69"/>
+      <c r="AU1" s="67">
         <v>42122</v>
       </c>
-      <c r="AV1" s="75"/>
-      <c r="AW1" s="75"/>
-      <c r="AX1" s="76"/>
-      <c r="AY1" s="74">
+      <c r="AV1" s="68"/>
+      <c r="AW1" s="68"/>
+      <c r="AX1" s="69"/>
+      <c r="AY1" s="67">
         <v>42129</v>
       </c>
-      <c r="AZ1" s="75"/>
-      <c r="BA1" s="75"/>
-      <c r="BB1" s="76"/>
-      <c r="BC1" s="74">
+      <c r="AZ1" s="68"/>
+      <c r="BA1" s="68"/>
+      <c r="BB1" s="69"/>
+      <c r="BC1" s="67">
         <v>42136</v>
       </c>
-      <c r="BD1" s="75"/>
-      <c r="BE1" s="75"/>
-      <c r="BF1" s="76"/>
-      <c r="BG1" s="74">
+      <c r="BD1" s="68"/>
+      <c r="BE1" s="68"/>
+      <c r="BF1" s="69"/>
+      <c r="BG1" s="67">
         <v>42143</v>
       </c>
-      <c r="BH1" s="75"/>
-      <c r="BI1" s="75"/>
-      <c r="BJ1" s="76"/>
-      <c r="BK1" s="74">
+      <c r="BH1" s="68"/>
+      <c r="BI1" s="68"/>
+      <c r="BJ1" s="69"/>
+      <c r="BK1" s="67">
         <v>42150</v>
       </c>
-      <c r="BL1" s="75"/>
-      <c r="BM1" s="75"/>
-      <c r="BN1" s="76"/>
-      <c r="BO1" s="74">
+      <c r="BL1" s="68"/>
+      <c r="BM1" s="68"/>
+      <c r="BN1" s="69"/>
+      <c r="BO1" s="67">
         <v>42157</v>
       </c>
-      <c r="BP1" s="75"/>
-      <c r="BQ1" s="75"/>
-      <c r="BR1" s="76"/>
+      <c r="BP1" s="68"/>
+      <c r="BQ1" s="68"/>
+      <c r="BR1" s="69"/>
       <c r="BS1" s="9"/>
     </row>
-    <row r="2" spans="1:73" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89"/>
+    <row r="2" spans="1:73" s="1" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="70"/>
       <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
@@ -1738,18 +1738,18 @@
       <c r="BT2" s="4"/>
       <c r="BU2" s="4"/>
     </row>
-    <row r="3" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="66">
         <v>1</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="79" t="s">
         <v>37</v>
       </c>
       <c r="C3" s="59"/>
-      <c r="D3" s="67">
+      <c r="D3" s="77">
         <v>4</v>
       </c>
-      <c r="E3" s="67"/>
+      <c r="E3" s="77"/>
       <c r="F3" s="38" t="s">
         <v>1</v>
       </c>
@@ -1791,12 +1791,12 @@
       <c r="BR3" s="12"/>
       <c r="BS3" s="10"/>
     </row>
-    <row r="4" spans="1:73" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:73" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="66"/>
-      <c r="B4" s="78"/>
+      <c r="B4" s="80"/>
       <c r="C4" s="60"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
       <c r="F4" s="39" t="s">
         <v>2</v>
       </c>
@@ -1870,20 +1870,20 @@
       <c r="BR4" s="15"/>
       <c r="BS4" s="13"/>
     </row>
-    <row r="5" spans="1:73" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:73" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="66">
         <v>2</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="71" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="79">
+      <c r="D5" s="81">
         <v>4</v>
       </c>
-      <c r="E5" s="72"/>
+      <c r="E5" s="71"/>
       <c r="F5" s="31" t="s">
         <v>1</v>
       </c>
@@ -1926,12 +1926,12 @@
       <c r="BR5" s="19"/>
       <c r="BS5" s="17"/>
     </row>
-    <row r="6" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="66"/>
-      <c r="B6" s="73"/>
+      <c r="B6" s="72"/>
       <c r="C6" s="63"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
       <c r="F6" s="32" t="s">
         <v>2</v>
       </c>
@@ -2005,20 +2005,20 @@
       <c r="BR6" s="22"/>
       <c r="BS6" s="20"/>
     </row>
-    <row r="7" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="66">
         <v>3</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="77" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="69">
+      <c r="D7" s="83">
         <v>4</v>
       </c>
-      <c r="E7" s="70"/>
+      <c r="E7" s="84"/>
       <c r="F7" s="29" t="s">
         <v>1</v>
       </c>
@@ -2061,12 +2061,12 @@
       <c r="BR7" s="12"/>
       <c r="BS7" s="10"/>
     </row>
-    <row r="8" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="66"/>
-      <c r="B8" s="68"/>
+      <c r="B8" s="78"/>
       <c r="C8" s="56"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="71"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="85"/>
       <c r="F8" s="30" t="s">
         <v>2</v>
       </c>
@@ -2142,20 +2142,20 @@
       <c r="BR8" s="15"/>
       <c r="BS8" s="13"/>
     </row>
-    <row r="9" spans="1:73" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:73" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="66">
         <v>7</v>
       </c>
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="71" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="79">
+      <c r="D9" s="81">
         <v>6</v>
       </c>
-      <c r="E9" s="72"/>
+      <c r="E9" s="71"/>
       <c r="F9" s="31" t="s">
         <v>1</v>
       </c>
@@ -2200,12 +2200,12 @@
       <c r="BR9" s="19"/>
       <c r="BS9" s="17"/>
     </row>
-    <row r="10" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="66"/>
-      <c r="B10" s="73"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="58"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
       <c r="F10" s="32" t="s">
         <v>2</v>
       </c>
@@ -2281,18 +2281,18 @@
       <c r="BR10" s="22"/>
       <c r="BS10" s="20"/>
     </row>
-    <row r="11" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="66">
         <v>4</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="77" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="65"/>
-      <c r="D11" s="69">
-        <v>1</v>
-      </c>
-      <c r="E11" s="70"/>
+      <c r="D11" s="83">
+        <v>1</v>
+      </c>
+      <c r="E11" s="84"/>
       <c r="F11" s="29" t="s">
         <v>1</v>
       </c>
@@ -2333,12 +2333,12 @@
       <c r="BR11" s="12"/>
       <c r="BS11" s="10"/>
     </row>
-    <row r="12" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="66"/>
-      <c r="B12" s="68"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="56"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="71"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="85"/>
       <c r="F12" s="30" t="s">
         <v>2</v>
       </c>
@@ -2410,20 +2410,20 @@
       <c r="BR12" s="15"/>
       <c r="BS12" s="13"/>
     </row>
-    <row r="13" spans="1:73" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:73" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="66">
         <v>5</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="71" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="72">
+      <c r="D13" s="71">
         <v>4</v>
       </c>
-      <c r="E13" s="72"/>
+      <c r="E13" s="71"/>
       <c r="F13" s="31" t="s">
         <v>1</v>
       </c>
@@ -2466,12 +2466,12 @@
       <c r="BR13" s="19"/>
       <c r="BS13" s="17"/>
     </row>
-    <row r="14" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="66"/>
-      <c r="B14" s="88"/>
+      <c r="B14" s="86"/>
       <c r="C14" s="64"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
       <c r="F14" s="32" t="s">
         <v>2</v>
       </c>
@@ -2501,7 +2501,9 @@
       <c r="AD14" s="22">
         <v>2</v>
       </c>
-      <c r="AE14" s="20"/>
+      <c r="AE14" s="20">
+        <v>2</v>
+      </c>
       <c r="AF14" s="21"/>
       <c r="AG14" s="21"/>
       <c r="AH14" s="22"/>
@@ -2543,20 +2545,20 @@
       <c r="BR14" s="22"/>
       <c r="BS14" s="20"/>
     </row>
-    <row r="15" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="66">
         <v>6</v>
       </c>
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="77" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="67">
+      <c r="D15" s="77">
         <v>3</v>
       </c>
-      <c r="E15" s="67"/>
+      <c r="E15" s="77"/>
       <c r="F15" s="29" t="s">
         <v>1</v>
       </c>
@@ -2599,12 +2601,12 @@
       <c r="BR15" s="12"/>
       <c r="BS15" s="10"/>
     </row>
-    <row r="16" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="66"/>
-      <c r="B16" s="68"/>
+      <c r="B16" s="78"/>
       <c r="C16" s="56"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
       <c r="F16" s="30" t="s">
         <v>2</v>
       </c>
@@ -2633,9 +2635,15 @@
       <c r="AC16" s="14"/>
       <c r="AD16" s="15"/>
       <c r="AE16" s="13"/>
-      <c r="AF16" s="14"/>
-      <c r="AG16" s="14"/>
-      <c r="AH16" s="15"/>
+      <c r="AF16" s="14">
+        <v>2</v>
+      </c>
+      <c r="AG16" s="14">
+        <v>2</v>
+      </c>
+      <c r="AH16" s="15">
+        <v>2</v>
+      </c>
       <c r="AI16" s="13"/>
       <c r="AJ16" s="14"/>
       <c r="AK16" s="14"/>
@@ -2674,18 +2682,18 @@
       <c r="BR16" s="15"/>
       <c r="BS16" s="13"/>
     </row>
-    <row r="17" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="66">
         <v>7</v>
       </c>
-      <c r="B17" s="72" t="s">
+      <c r="B17" s="71" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="57"/>
-      <c r="D17" s="79">
+      <c r="D17" s="81">
         <v>4</v>
       </c>
-      <c r="E17" s="72"/>
+      <c r="E17" s="71"/>
       <c r="F17" s="31" t="s">
         <v>1</v>
       </c>
@@ -2728,12 +2736,12 @@
       <c r="BR17" s="19"/>
       <c r="BS17" s="17"/>
     </row>
-    <row r="18" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="66"/>
-      <c r="B18" s="73"/>
+      <c r="B18" s="72"/>
       <c r="C18" s="58"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
       <c r="F18" s="32" t="s">
         <v>2</v>
       </c>
@@ -2803,7 +2811,7 @@
       <c r="BR18" s="22"/>
       <c r="BS18" s="20"/>
     </row>
-    <row r="19" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="66">
         <v>8</v>
       </c>
@@ -2813,10 +2821,10 @@
       <c r="C19" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="67">
+      <c r="D19" s="77">
         <v>8</v>
       </c>
-      <c r="E19" s="67"/>
+      <c r="E19" s="77"/>
       <c r="F19" s="29" t="s">
         <v>1</v>
       </c>
@@ -2864,14 +2872,14 @@
       <c r="BR19" s="12"/>
       <c r="BS19" s="10"/>
     </row>
-    <row r="20" spans="1:71" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:71" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="66"/>
       <c r="B20" s="52" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="56"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
       <c r="F20" s="30" t="s">
         <v>2</v>
       </c>
@@ -2941,20 +2949,20 @@
       <c r="BR20" s="15"/>
       <c r="BS20" s="13"/>
     </row>
-    <row r="21" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="66">
         <v>7</v>
       </c>
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="71" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="79">
+      <c r="D21" s="81">
         <v>4</v>
       </c>
-      <c r="E21" s="80"/>
+      <c r="E21" s="87"/>
       <c r="F21" s="31" t="s">
         <v>1</v>
       </c>
@@ -2997,12 +3005,12 @@
       <c r="BR21" s="19"/>
       <c r="BS21" s="17"/>
     </row>
-    <row r="22" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="66"/>
-      <c r="B22" s="73"/>
+      <c r="B22" s="72"/>
       <c r="C22" s="58"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="82"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="89"/>
       <c r="F22" s="32" t="s">
         <v>2</v>
       </c>
@@ -3072,20 +3080,20 @@
       <c r="BR22" s="22"/>
       <c r="BS22" s="20"/>
     </row>
-    <row r="23" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="66">
         <v>8</v>
       </c>
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="77" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="67">
+      <c r="D23" s="77">
         <v>4</v>
       </c>
-      <c r="E23" s="67"/>
+      <c r="E23" s="77"/>
       <c r="F23" s="29" t="s">
         <v>1</v>
       </c>
@@ -3128,12 +3136,12 @@
       <c r="BR23" s="12"/>
       <c r="BS23" s="10"/>
     </row>
-    <row r="24" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="66"/>
-      <c r="B24" s="68"/>
+      <c r="B24" s="78"/>
       <c r="C24" s="56"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
+      <c r="D24" s="78"/>
+      <c r="E24" s="78"/>
       <c r="F24" s="30" t="s">
         <v>2</v>
       </c>
@@ -3203,20 +3211,20 @@
       <c r="BR24" s="15"/>
       <c r="BS24" s="13"/>
     </row>
-    <row r="25" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="66">
         <v>7</v>
       </c>
-      <c r="B25" s="72" t="s">
+      <c r="B25" s="71" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="79">
+      <c r="D25" s="81">
         <v>4</v>
       </c>
-      <c r="E25" s="72"/>
+      <c r="E25" s="71"/>
       <c r="F25" s="31" t="s">
         <v>1</v>
       </c>
@@ -3259,12 +3267,12 @@
       <c r="BR25" s="19"/>
       <c r="BS25" s="17"/>
     </row>
-    <row r="26" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="66"/>
-      <c r="B26" s="73"/>
+      <c r="B26" s="72"/>
       <c r="C26" s="58"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
       <c r="F26" s="32" t="s">
         <v>2</v>
       </c>
@@ -3334,20 +3342,20 @@
       <c r="BR26" s="22"/>
       <c r="BS26" s="20"/>
     </row>
-    <row r="27" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="66">
         <v>8</v>
       </c>
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="77" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="67">
+      <c r="D27" s="77">
         <v>4</v>
       </c>
-      <c r="E27" s="67"/>
+      <c r="E27" s="77"/>
       <c r="F27" s="29" t="s">
         <v>1</v>
       </c>
@@ -3390,12 +3398,12 @@
       <c r="BR27" s="12"/>
       <c r="BS27" s="10"/>
     </row>
-    <row r="28" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="66"/>
-      <c r="B28" s="68"/>
+      <c r="B28" s="78"/>
       <c r="C28" s="56"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
       <c r="F28" s="30" t="s">
         <v>2</v>
       </c>
@@ -3465,20 +3473,20 @@
       <c r="BR28" s="15"/>
       <c r="BS28" s="13"/>
     </row>
-    <row r="29" spans="1:71" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:71" s="18" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="66">
         <v>9</v>
       </c>
-      <c r="B29" s="72" t="s">
+      <c r="B29" s="71" t="s">
         <v>51</v>
       </c>
       <c r="C29" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="72">
+      <c r="D29" s="71">
         <v>12</v>
       </c>
-      <c r="E29" s="72"/>
+      <c r="E29" s="71"/>
       <c r="F29" s="31" t="s">
         <v>1</v>
       </c>
@@ -3546,12 +3554,12 @@
       <c r="BR29" s="19"/>
       <c r="BS29" s="17"/>
     </row>
-    <row r="30" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="66"/>
-      <c r="B30" s="73"/>
+      <c r="B30" s="72"/>
       <c r="C30" s="58"/>
-      <c r="D30" s="73"/>
-      <c r="E30" s="73"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="72"/>
       <c r="F30" s="32" t="s">
         <v>2</v>
       </c>
@@ -3621,18 +3629,18 @@
       <c r="BR30" s="22"/>
       <c r="BS30" s="20"/>
     </row>
-    <row r="31" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="66">
         <v>10</v>
       </c>
-      <c r="B31" s="67" t="s">
+      <c r="B31" s="77" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="55"/>
-      <c r="D31" s="67">
+      <c r="D31" s="77">
         <v>8</v>
       </c>
-      <c r="E31" s="67"/>
+      <c r="E31" s="77"/>
       <c r="F31" s="29" t="s">
         <v>1</v>
       </c>
@@ -3680,12 +3688,12 @@
       <c r="BR31" s="12"/>
       <c r="BS31" s="10"/>
     </row>
-    <row r="32" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="66"/>
-      <c r="B32" s="68"/>
+      <c r="B32" s="78"/>
       <c r="C32" s="56"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="68"/>
+      <c r="D32" s="78"/>
+      <c r="E32" s="78"/>
       <c r="F32" s="30" t="s">
         <v>2</v>
       </c>
@@ -3755,18 +3763,18 @@
       <c r="BR32" s="15"/>
       <c r="BS32" s="13"/>
     </row>
-    <row r="33" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="66">
         <v>11</v>
       </c>
-      <c r="B33" s="72" t="s">
+      <c r="B33" s="71" t="s">
         <v>24</v>
       </c>
       <c r="C33" s="57"/>
-      <c r="D33" s="72">
+      <c r="D33" s="71">
         <v>8</v>
       </c>
-      <c r="E33" s="72"/>
+      <c r="E33" s="71"/>
       <c r="F33" s="31" t="s">
         <v>1</v>
       </c>
@@ -3854,12 +3862,12 @@
       <c r="BR33" s="19"/>
       <c r="BS33" s="17"/>
     </row>
-    <row r="34" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="66"/>
-      <c r="B34" s="73"/>
+      <c r="B34" s="72"/>
       <c r="C34" s="58"/>
-      <c r="D34" s="73"/>
-      <c r="E34" s="73"/>
+      <c r="D34" s="72"/>
+      <c r="E34" s="72"/>
       <c r="F34" s="32" t="s">
         <v>2</v>
       </c>
@@ -3929,18 +3937,18 @@
       <c r="BR34" s="22"/>
       <c r="BS34" s="20"/>
     </row>
-    <row r="35" spans="1:71" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:71" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="66">
         <v>12</v>
       </c>
-      <c r="B35" s="77" t="s">
+      <c r="B35" s="79" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="59"/>
-      <c r="D35" s="67">
+      <c r="D35" s="77">
         <v>2</v>
       </c>
-      <c r="E35" s="67"/>
+      <c r="E35" s="77"/>
       <c r="F35" s="29" t="s">
         <v>1</v>
       </c>
@@ -3980,12 +3988,12 @@
       <c r="BR35" s="12"/>
       <c r="BS35" s="10"/>
     </row>
-    <row r="36" spans="1:71" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:71" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="66"/>
-      <c r="B36" s="78"/>
+      <c r="B36" s="80"/>
       <c r="C36" s="60"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="68"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
       <c r="F36" s="30" t="s">
         <v>2</v>
       </c>
@@ -4055,18 +4063,18 @@
       <c r="BR36" s="15"/>
       <c r="BS36" s="13"/>
     </row>
-    <row r="37" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="66">
         <v>13</v>
       </c>
-      <c r="B37" s="72" t="s">
+      <c r="B37" s="71" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="57"/>
-      <c r="D37" s="72">
+      <c r="D37" s="71">
         <v>6</v>
       </c>
-      <c r="E37" s="72"/>
+      <c r="E37" s="71"/>
       <c r="F37" s="31" t="s">
         <v>1</v>
       </c>
@@ -4117,12 +4125,12 @@
       <c r="BR37" s="19"/>
       <c r="BS37" s="17"/>
     </row>
-    <row r="38" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="66"/>
-      <c r="B38" s="73"/>
+      <c r="B38" s="72"/>
       <c r="C38" s="58"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="73"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="72"/>
       <c r="F38" s="32" t="s">
         <v>2</v>
       </c>
@@ -4192,18 +4200,18 @@
       <c r="BR38" s="22"/>
       <c r="BS38" s="20"/>
     </row>
-    <row r="39" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="66">
         <v>14</v>
       </c>
-      <c r="B39" s="67" t="s">
+      <c r="B39" s="77" t="s">
         <v>39</v>
       </c>
       <c r="C39" s="55"/>
-      <c r="D39" s="67">
+      <c r="D39" s="77">
         <v>4</v>
       </c>
-      <c r="E39" s="67"/>
+      <c r="E39" s="77"/>
       <c r="F39" s="29" t="s">
         <v>1</v>
       </c>
@@ -4251,12 +4259,12 @@
       <c r="BR39" s="12"/>
       <c r="BS39" s="10"/>
     </row>
-    <row r="40" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="66"/>
-      <c r="B40" s="68"/>
+      <c r="B40" s="78"/>
       <c r="C40" s="56"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="68"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="78"/>
       <c r="F40" s="30" t="s">
         <v>2</v>
       </c>
@@ -4326,14 +4334,14 @@
       <c r="BR40" s="15"/>
       <c r="BS40" s="13"/>
     </row>
-    <row r="41" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="66">
         <v>15</v>
       </c>
-      <c r="B41" s="72"/>
+      <c r="B41" s="71"/>
       <c r="C41" s="57"/>
-      <c r="D41" s="72"/>
-      <c r="E41" s="72"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
       <c r="F41" s="31" t="s">
         <v>1</v>
       </c>
@@ -4371,12 +4379,12 @@
       <c r="BR41" s="19"/>
       <c r="BS41" s="17"/>
     </row>
-    <row r="42" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="66"/>
-      <c r="B42" s="73"/>
+      <c r="B42" s="72"/>
       <c r="C42" s="58"/>
-      <c r="D42" s="73"/>
-      <c r="E42" s="73"/>
+      <c r="D42" s="72"/>
+      <c r="E42" s="72"/>
       <c r="F42" s="32" t="s">
         <v>2</v>
       </c>
@@ -4446,7 +4454,7 @@
       <c r="BR42" s="22"/>
       <c r="BS42" s="20"/>
     </row>
-    <row r="43" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="66">
         <v>16</v>
       </c>
@@ -4491,7 +4499,7 @@
       <c r="BR43" s="12"/>
       <c r="BS43" s="10"/>
     </row>
-    <row r="44" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="66"/>
       <c r="B44" s="50"/>
       <c r="C44" s="60"/>
@@ -4566,16 +4574,16 @@
       <c r="BR44" s="15"/>
       <c r="BS44" s="13"/>
     </row>
-    <row r="45" spans="1:71" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:71" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A45" s="66">
         <v>18</v>
       </c>
-      <c r="B45" s="83" t="s">
+      <c r="B45" s="73" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="61"/>
-      <c r="D45" s="85"/>
-      <c r="E45" s="85"/>
+      <c r="D45" s="75"/>
+      <c r="E45" s="75"/>
       <c r="F45" s="40"/>
       <c r="G45" s="41"/>
       <c r="H45" s="42"/>
@@ -4663,12 +4671,12 @@
       <c r="BR45" s="43"/>
       <c r="BS45" s="10"/>
     </row>
-    <row r="46" spans="1:71" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:71" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A46" s="66"/>
-      <c r="B46" s="84"/>
+      <c r="B46" s="74"/>
       <c r="C46" s="62"/>
-      <c r="D46" s="86"/>
-      <c r="E46" s="86"/>
+      <c r="D46" s="76"/>
+      <c r="E46" s="76"/>
       <c r="F46" s="44"/>
       <c r="G46" s="45"/>
       <c r="H46" s="46"/>
@@ -4736,16 +4744,16 @@
       <c r="BR46" s="47"/>
       <c r="BS46" s="13"/>
     </row>
-    <row r="47" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="66">
         <v>19</v>
       </c>
-      <c r="B47" s="72" t="s">
+      <c r="B47" s="71" t="s">
         <v>40</v>
       </c>
       <c r="C47" s="57"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="72"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="71"/>
       <c r="F47" s="31"/>
       <c r="G47" s="17"/>
       <c r="J47" s="19"/>
@@ -4781,12 +4789,12 @@
       <c r="BR47" s="19"/>
       <c r="BS47" s="17"/>
     </row>
-    <row r="48" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="66"/>
-      <c r="B48" s="73"/>
+      <c r="B48" s="72"/>
       <c r="C48" s="58"/>
-      <c r="D48" s="73"/>
-      <c r="E48" s="73"/>
+      <c r="D48" s="72"/>
+      <c r="E48" s="72"/>
       <c r="F48" s="32"/>
       <c r="G48" s="20"/>
       <c r="H48" s="21"/>
@@ -4854,16 +4862,16 @@
       <c r="BR48" s="22"/>
       <c r="BS48" s="20"/>
     </row>
-    <row r="49" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="66">
         <v>20</v>
       </c>
-      <c r="B49" s="67" t="s">
+      <c r="B49" s="77" t="s">
         <v>41</v>
       </c>
       <c r="C49" s="55"/>
-      <c r="D49" s="67"/>
-      <c r="E49" s="67"/>
+      <c r="D49" s="77"/>
+      <c r="E49" s="77"/>
       <c r="F49" s="29"/>
       <c r="G49" s="10"/>
       <c r="J49" s="12"/>
@@ -4899,12 +4907,12 @@
       <c r="BR49" s="12"/>
       <c r="BS49" s="10"/>
     </row>
-    <row r="50" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="66"/>
-      <c r="B50" s="68"/>
+      <c r="B50" s="78"/>
       <c r="C50" s="56"/>
-      <c r="D50" s="68"/>
-      <c r="E50" s="68"/>
+      <c r="D50" s="78"/>
+      <c r="E50" s="78"/>
       <c r="F50" s="30"/>
       <c r="G50" s="13"/>
       <c r="H50" s="14"/>
@@ -4972,16 +4980,16 @@
       <c r="BR50" s="15"/>
       <c r="BS50" s="13"/>
     </row>
-    <row r="51" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="66">
         <v>21</v>
       </c>
-      <c r="B51" s="72" t="s">
+      <c r="B51" s="71" t="s">
         <v>42</v>
       </c>
       <c r="C51" s="57"/>
-      <c r="D51" s="72"/>
-      <c r="E51" s="72"/>
+      <c r="D51" s="71"/>
+      <c r="E51" s="71"/>
       <c r="F51" s="31"/>
       <c r="G51" s="17"/>
       <c r="J51" s="19"/>
@@ -5017,12 +5025,12 @@
       <c r="BR51" s="19"/>
       <c r="BS51" s="17"/>
     </row>
-    <row r="52" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="66"/>
-      <c r="B52" s="73"/>
+      <c r="B52" s="72"/>
       <c r="C52" s="58"/>
-      <c r="D52" s="73"/>
-      <c r="E52" s="73"/>
+      <c r="D52" s="72"/>
+      <c r="E52" s="72"/>
       <c r="F52" s="32"/>
       <c r="G52" s="20"/>
       <c r="H52" s="21"/>
@@ -5090,16 +5098,16 @@
       <c r="BR52" s="22"/>
       <c r="BS52" s="20"/>
     </row>
-    <row r="53" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="66">
         <v>22</v>
       </c>
-      <c r="B53" s="67" t="s">
+      <c r="B53" s="77" t="s">
         <v>43</v>
       </c>
       <c r="C53" s="55"/>
-      <c r="D53" s="67"/>
-      <c r="E53" s="67"/>
+      <c r="D53" s="77"/>
+      <c r="E53" s="77"/>
       <c r="F53" s="29"/>
       <c r="G53" s="10"/>
       <c r="J53" s="12"/>
@@ -5135,12 +5143,12 @@
       <c r="BR53" s="12"/>
       <c r="BS53" s="10"/>
     </row>
-    <row r="54" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="66"/>
-      <c r="B54" s="68"/>
+      <c r="B54" s="78"/>
       <c r="C54" s="56"/>
-      <c r="D54" s="68"/>
-      <c r="E54" s="68"/>
+      <c r="D54" s="78"/>
+      <c r="E54" s="78"/>
       <c r="F54" s="30"/>
       <c r="G54" s="13"/>
       <c r="H54" s="14"/>
@@ -5208,16 +5216,16 @@
       <c r="BR54" s="15"/>
       <c r="BS54" s="13"/>
     </row>
-    <row r="55" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="66">
         <v>23</v>
       </c>
-      <c r="B55" s="72" t="s">
+      <c r="B55" s="71" t="s">
         <v>44</v>
       </c>
       <c r="C55" s="57"/>
-      <c r="D55" s="72"/>
-      <c r="E55" s="72"/>
+      <c r="D55" s="71"/>
+      <c r="E55" s="71"/>
       <c r="F55" s="31"/>
       <c r="G55" s="17"/>
       <c r="J55" s="19"/>
@@ -5253,12 +5261,12 @@
       <c r="BR55" s="19"/>
       <c r="BS55" s="17"/>
     </row>
-    <row r="56" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="66"/>
-      <c r="B56" s="73"/>
+      <c r="B56" s="72"/>
       <c r="C56" s="58"/>
-      <c r="D56" s="73"/>
-      <c r="E56" s="73"/>
+      <c r="D56" s="72"/>
+      <c r="E56" s="72"/>
       <c r="F56" s="32"/>
       <c r="G56" s="20"/>
       <c r="H56" s="21"/>
@@ -5326,16 +5334,16 @@
       <c r="BR56" s="22"/>
       <c r="BS56" s="20"/>
     </row>
-    <row r="57" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="66">
         <v>24</v>
       </c>
-      <c r="B57" s="67" t="s">
+      <c r="B57" s="77" t="s">
         <v>45</v>
       </c>
       <c r="C57" s="55"/>
-      <c r="D57" s="67"/>
-      <c r="E57" s="67"/>
+      <c r="D57" s="77"/>
+      <c r="E57" s="77"/>
       <c r="F57" s="29"/>
       <c r="G57" s="10"/>
       <c r="J57" s="12"/>
@@ -5371,12 +5379,12 @@
       <c r="BR57" s="12"/>
       <c r="BS57" s="10"/>
     </row>
-    <row r="58" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="66"/>
-      <c r="B58" s="68"/>
+      <c r="B58" s="78"/>
       <c r="C58" s="56"/>
-      <c r="D58" s="68"/>
-      <c r="E58" s="68"/>
+      <c r="D58" s="78"/>
+      <c r="E58" s="78"/>
       <c r="F58" s="30"/>
       <c r="G58" s="13"/>
       <c r="H58" s="14"/>
@@ -5444,16 +5452,16 @@
       <c r="BR58" s="15"/>
       <c r="BS58" s="13"/>
     </row>
-    <row r="59" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="66">
         <v>25</v>
       </c>
-      <c r="B59" s="72" t="s">
+      <c r="B59" s="71" t="s">
         <v>46</v>
       </c>
       <c r="C59" s="57"/>
-      <c r="D59" s="72"/>
-      <c r="E59" s="72"/>
+      <c r="D59" s="71"/>
+      <c r="E59" s="71"/>
       <c r="F59" s="31"/>
       <c r="G59" s="17"/>
       <c r="J59" s="19"/>
@@ -5489,12 +5497,12 @@
       <c r="BR59" s="19"/>
       <c r="BS59" s="17"/>
     </row>
-    <row r="60" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="66"/>
-      <c r="B60" s="73"/>
+      <c r="B60" s="72"/>
       <c r="C60" s="58"/>
-      <c r="D60" s="73"/>
-      <c r="E60" s="73"/>
+      <c r="D60" s="72"/>
+      <c r="E60" s="72"/>
       <c r="F60" s="32"/>
       <c r="G60" s="20"/>
       <c r="H60" s="21"/>
@@ -5562,16 +5570,16 @@
       <c r="BR60" s="22"/>
       <c r="BS60" s="20"/>
     </row>
-    <row r="61" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="66">
         <v>26</v>
       </c>
-      <c r="B61" s="67" t="s">
+      <c r="B61" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C61" s="55"/>
-      <c r="D61" s="67"/>
-      <c r="E61" s="67"/>
+      <c r="D61" s="77"/>
+      <c r="E61" s="77"/>
       <c r="F61" s="29"/>
       <c r="G61" s="10"/>
       <c r="J61" s="12"/>
@@ -5607,12 +5615,12 @@
       <c r="BR61" s="12"/>
       <c r="BS61" s="10"/>
     </row>
-    <row r="62" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="66"/>
-      <c r="B62" s="68"/>
+      <c r="B62" s="78"/>
       <c r="C62" s="56"/>
-      <c r="D62" s="68"/>
-      <c r="E62" s="68"/>
+      <c r="D62" s="78"/>
+      <c r="E62" s="78"/>
       <c r="F62" s="30"/>
       <c r="G62" s="13"/>
       <c r="H62" s="14"/>
@@ -5680,16 +5688,16 @@
       <c r="BR62" s="15"/>
       <c r="BS62" s="13"/>
     </row>
-    <row r="63" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="66">
         <v>27</v>
       </c>
-      <c r="B63" s="72" t="s">
+      <c r="B63" s="71" t="s">
         <v>48</v>
       </c>
       <c r="C63" s="57"/>
-      <c r="D63" s="72"/>
-      <c r="E63" s="72"/>
+      <c r="D63" s="71"/>
+      <c r="E63" s="71"/>
       <c r="F63" s="31"/>
       <c r="G63" s="17"/>
       <c r="J63" s="19"/>
@@ -5725,12 +5733,12 @@
       <c r="BR63" s="19"/>
       <c r="BS63" s="17"/>
     </row>
-    <row r="64" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="66"/>
-      <c r="B64" s="73"/>
+      <c r="B64" s="72"/>
       <c r="C64" s="58"/>
-      <c r="D64" s="73"/>
-      <c r="E64" s="73"/>
+      <c r="D64" s="72"/>
+      <c r="E64" s="72"/>
       <c r="F64" s="32"/>
       <c r="G64" s="20"/>
       <c r="H64" s="21"/>
@@ -5798,16 +5806,16 @@
       <c r="BR64" s="22"/>
       <c r="BS64" s="20"/>
     </row>
-    <row r="65" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="66">
         <v>28</v>
       </c>
-      <c r="B65" s="67" t="s">
+      <c r="B65" s="77" t="s">
         <v>49</v>
       </c>
       <c r="C65" s="55"/>
-      <c r="D65" s="67"/>
-      <c r="E65" s="67"/>
+      <c r="D65" s="77"/>
+      <c r="E65" s="77"/>
       <c r="F65" s="29"/>
       <c r="G65" s="10"/>
       <c r="J65" s="12"/>
@@ -5843,12 +5851,12 @@
       <c r="BR65" s="12"/>
       <c r="BS65" s="10"/>
     </row>
-    <row r="66" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="66"/>
-      <c r="B66" s="68"/>
+      <c r="B66" s="78"/>
       <c r="C66" s="56"/>
-      <c r="D66" s="68"/>
-      <c r="E66" s="68"/>
+      <c r="D66" s="78"/>
+      <c r="E66" s="78"/>
       <c r="F66" s="33"/>
       <c r="G66" s="13"/>
       <c r="H66" s="14"/>
@@ -5916,7 +5924,7 @@
       <c r="BR66" s="15"/>
       <c r="BS66" s="13"/>
     </row>
-    <row r="67" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:71" x14ac:dyDescent="0.35">
       <c r="B67" s="6" t="s">
         <v>12</v>
       </c>
@@ -5926,6 +5934,92 @@
     </row>
   </sheetData>
   <mergeCells count="110">
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:E50"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D27:E28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D29:E30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="D31:E32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="D17:E18"/>
+    <mergeCell ref="BC1:BF1"/>
+    <mergeCell ref="BG1:BJ1"/>
+    <mergeCell ref="BK1:BN1"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="D47:E48"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D33:E34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="D35:E36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:E38"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D39:E40"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="D19:E20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D21:E22"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:E24"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:E10"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="D41:E42"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D25:E26"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="D63:E64"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D45:E46"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="D65:E66"/>
+    <mergeCell ref="D51:E52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:E54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="D55:E56"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="D57:E58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="D59:E60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="D61:E62"/>
     <mergeCell ref="A63:A64"/>
     <mergeCell ref="A65:A66"/>
     <mergeCell ref="A55:A56"/>
@@ -5950,92 +6044,6 @@
     <mergeCell ref="AE1:AH1"/>
     <mergeCell ref="W1:Z1"/>
     <mergeCell ref="AA1:AD1"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="D63:E64"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D45:E46"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="D65:E66"/>
-    <mergeCell ref="D51:E52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:E54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="D55:E56"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="D57:E58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="D59:E60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="D61:E62"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:E24"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:E10"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="D41:E42"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:E6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:E12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D13:E14"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D25:E26"/>
-    <mergeCell ref="BC1:BF1"/>
-    <mergeCell ref="BG1:BJ1"/>
-    <mergeCell ref="BK1:BN1"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="D47:E48"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="D33:E34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="D35:E36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:E38"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:E40"/>
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="D19:E20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D21:E22"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:E50"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:E8"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="D27:E28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D29:E30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="D31:E32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="D17:E18"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:BR8 G25:BR44 G11:BR16 G46:BR64 G45:AW45 BD45:BR45 AY45:BB45">
     <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">

</xml_diff>

<commit_message>
some long ago changes to element list
</commit_message>
<xml_diff>
--- a/doc/Projektplan Gantt.xlsx
+++ b/doc/Projektplan Gantt.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="25610" windowHeight="16010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14000"/>
   </bookViews>
   <sheets>
     <sheet name="Balkenplan" sheetId="1" r:id="rId1"/>
@@ -779,6 +779,30 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -788,13 +812,25 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -809,82 +845,46 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="60 % - Akzent1" xfId="2" builtinId="32"/>
     <cellStyle name="Akzent1" xfId="1" builtinId="29"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
@@ -1355,73 +1355,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AG16" sqref="AG16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="47.7265625" customWidth="1"/>
-    <col min="4" max="5" width="12.7265625" customWidth="1"/>
-    <col min="6" max="6" width="4.453125" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.1796875" style="5" customWidth="1"/>
-    <col min="8" max="9" width="3.1796875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="3.1796875" style="8" customWidth="1"/>
-    <col min="11" max="11" width="3.1796875" style="5" customWidth="1"/>
-    <col min="12" max="13" width="3.1796875" style="6" customWidth="1"/>
-    <col min="14" max="14" width="3.1796875" style="8" customWidth="1"/>
-    <col min="15" max="15" width="3.1796875" style="5" customWidth="1"/>
-    <col min="16" max="17" width="3.1796875" style="6" customWidth="1"/>
-    <col min="18" max="18" width="3.1796875" style="8" customWidth="1"/>
-    <col min="19" max="19" width="3.1796875" style="5" customWidth="1"/>
-    <col min="20" max="21" width="3.1796875" style="6" customWidth="1"/>
-    <col min="22" max="22" width="3.1796875" style="8" customWidth="1"/>
-    <col min="23" max="23" width="3.1796875" style="5" customWidth="1"/>
-    <col min="24" max="25" width="3.1796875" style="6" customWidth="1"/>
-    <col min="26" max="26" width="3.1796875" style="8" customWidth="1"/>
-    <col min="27" max="27" width="3.1796875" style="5" customWidth="1"/>
-    <col min="28" max="29" width="3.1796875" style="6" customWidth="1"/>
-    <col min="30" max="30" width="3.1796875" style="8" customWidth="1"/>
-    <col min="31" max="31" width="3.1796875" style="5" customWidth="1"/>
-    <col min="32" max="33" width="3.1796875" style="6" customWidth="1"/>
-    <col min="34" max="34" width="3.1796875" style="8" customWidth="1"/>
-    <col min="35" max="35" width="3.1796875" style="5" customWidth="1"/>
-    <col min="36" max="37" width="3.1796875" style="6" customWidth="1"/>
-    <col min="38" max="38" width="3.1796875" style="8" customWidth="1"/>
-    <col min="39" max="39" width="3.1796875" style="5" customWidth="1"/>
-    <col min="40" max="41" width="3.1796875" style="6" customWidth="1"/>
-    <col min="42" max="42" width="3.1796875" style="8" customWidth="1"/>
-    <col min="43" max="43" width="3.1796875" style="5" customWidth="1"/>
-    <col min="44" max="45" width="3.1796875" style="6" customWidth="1"/>
-    <col min="46" max="46" width="3.1796875" style="8" customWidth="1"/>
-    <col min="47" max="47" width="3.1796875" style="5" customWidth="1"/>
-    <col min="48" max="49" width="3.1796875" style="6" customWidth="1"/>
-    <col min="50" max="50" width="3.1796875" style="8" customWidth="1"/>
-    <col min="51" max="51" width="3.1796875" style="5" customWidth="1"/>
-    <col min="52" max="53" width="3.1796875" style="6" customWidth="1"/>
-    <col min="54" max="54" width="3.1796875" style="8" customWidth="1"/>
-    <col min="55" max="55" width="3.1796875" style="5" customWidth="1"/>
-    <col min="56" max="57" width="3.1796875" style="6" customWidth="1"/>
-    <col min="58" max="58" width="3.1796875" style="8" customWidth="1"/>
-    <col min="59" max="59" width="3.1796875" style="5" customWidth="1"/>
-    <col min="60" max="61" width="3.1796875" style="6" customWidth="1"/>
-    <col min="62" max="62" width="3.1796875" style="8" customWidth="1"/>
-    <col min="63" max="63" width="3.1796875" style="5" customWidth="1"/>
-    <col min="64" max="65" width="3.1796875" style="6" customWidth="1"/>
-    <col min="66" max="66" width="3.1796875" style="8" customWidth="1"/>
-    <col min="67" max="67" width="3.1796875" style="5" customWidth="1"/>
-    <col min="68" max="69" width="3.1796875" style="6" customWidth="1"/>
-    <col min="70" max="70" width="3.1796875" style="8" customWidth="1"/>
-    <col min="71" max="71" width="3.1796875" style="5" customWidth="1"/>
-    <col min="72" max="72" width="2.7265625" customWidth="1"/>
-    <col min="73" max="73" width="2.453125" customWidth="1"/>
-    <col min="74" max="74" width="2.1796875" customWidth="1"/>
-    <col min="75" max="75" width="2.453125" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="47.6640625" customWidth="1"/>
+    <col min="4" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="4.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.1640625" style="5" customWidth="1"/>
+    <col min="8" max="9" width="3.1640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="3.1640625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="3.1640625" style="5" customWidth="1"/>
+    <col min="12" max="13" width="3.1640625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="3.1640625" style="8" customWidth="1"/>
+    <col min="15" max="15" width="3.1640625" style="5" customWidth="1"/>
+    <col min="16" max="17" width="3.1640625" style="6" customWidth="1"/>
+    <col min="18" max="18" width="3.1640625" style="8" customWidth="1"/>
+    <col min="19" max="19" width="3.1640625" style="5" customWidth="1"/>
+    <col min="20" max="21" width="3.1640625" style="6" customWidth="1"/>
+    <col min="22" max="22" width="3.1640625" style="8" customWidth="1"/>
+    <col min="23" max="23" width="3.1640625" style="5" customWidth="1"/>
+    <col min="24" max="25" width="3.1640625" style="6" customWidth="1"/>
+    <col min="26" max="26" width="3.1640625" style="8" customWidth="1"/>
+    <col min="27" max="27" width="3.1640625" style="5" customWidth="1"/>
+    <col min="28" max="29" width="3.1640625" style="6" customWidth="1"/>
+    <col min="30" max="30" width="3.1640625" style="8" customWidth="1"/>
+    <col min="31" max="31" width="3.1640625" style="5" customWidth="1"/>
+    <col min="32" max="33" width="3.1640625" style="6" customWidth="1"/>
+    <col min="34" max="34" width="3.1640625" style="8" customWidth="1"/>
+    <col min="35" max="35" width="3.1640625" style="5" customWidth="1"/>
+    <col min="36" max="37" width="3.1640625" style="6" customWidth="1"/>
+    <col min="38" max="38" width="3.1640625" style="8" customWidth="1"/>
+    <col min="39" max="39" width="3.1640625" style="5" customWidth="1"/>
+    <col min="40" max="41" width="3.1640625" style="6" customWidth="1"/>
+    <col min="42" max="42" width="3.1640625" style="8" customWidth="1"/>
+    <col min="43" max="43" width="3.1640625" style="5" customWidth="1"/>
+    <col min="44" max="45" width="3.1640625" style="6" customWidth="1"/>
+    <col min="46" max="46" width="3.1640625" style="8" customWidth="1"/>
+    <col min="47" max="47" width="3.1640625" style="5" customWidth="1"/>
+    <col min="48" max="49" width="3.1640625" style="6" customWidth="1"/>
+    <col min="50" max="50" width="3.1640625" style="8" customWidth="1"/>
+    <col min="51" max="51" width="3.1640625" style="5" customWidth="1"/>
+    <col min="52" max="53" width="3.1640625" style="6" customWidth="1"/>
+    <col min="54" max="54" width="3.1640625" style="8" customWidth="1"/>
+    <col min="55" max="55" width="3.1640625" style="5" customWidth="1"/>
+    <col min="56" max="57" width="3.1640625" style="6" customWidth="1"/>
+    <col min="58" max="58" width="3.1640625" style="8" customWidth="1"/>
+    <col min="59" max="59" width="3.1640625" style="5" customWidth="1"/>
+    <col min="60" max="61" width="3.1640625" style="6" customWidth="1"/>
+    <col min="62" max="62" width="3.1640625" style="8" customWidth="1"/>
+    <col min="63" max="63" width="3.1640625" style="5" customWidth="1"/>
+    <col min="64" max="65" width="3.1640625" style="6" customWidth="1"/>
+    <col min="66" max="66" width="3.1640625" style="8" customWidth="1"/>
+    <col min="67" max="67" width="3.1640625" style="5" customWidth="1"/>
+    <col min="68" max="69" width="3.1640625" style="6" customWidth="1"/>
+    <col min="70" max="70" width="3.1640625" style="8" customWidth="1"/>
+    <col min="71" max="71" width="3.1640625" style="5" customWidth="1"/>
+    <col min="72" max="72" width="2.6640625" customWidth="1"/>
+    <col min="73" max="73" width="2.5" customWidth="1"/>
+    <col min="74" max="74" width="2.1640625" customWidth="1"/>
+    <col min="75" max="75" width="2.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" s="2" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:73" s="2" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="26"/>
@@ -1431,106 +1431,106 @@
         <v>3</v>
       </c>
       <c r="F1" s="35"/>
-      <c r="G1" s="67">
+      <c r="G1" s="75">
         <v>42031</v>
       </c>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="67">
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="75">
         <v>42038</v>
       </c>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="67">
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="75">
         <v>42045</v>
       </c>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="67">
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="75">
         <v>42052</v>
       </c>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="67">
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="75">
         <v>42059</v>
       </c>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="69"/>
-      <c r="AA1" s="67">
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="75">
         <v>42066</v>
       </c>
-      <c r="AB1" s="68"/>
-      <c r="AC1" s="68"/>
-      <c r="AD1" s="69"/>
-      <c r="AE1" s="67">
+      <c r="AB1" s="76"/>
+      <c r="AC1" s="76"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="75">
         <v>42073</v>
       </c>
-      <c r="AF1" s="68"/>
-      <c r="AG1" s="68"/>
-      <c r="AH1" s="69"/>
-      <c r="AI1" s="67">
+      <c r="AF1" s="76"/>
+      <c r="AG1" s="76"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="75">
         <v>42080</v>
       </c>
-      <c r="AJ1" s="68"/>
-      <c r="AK1" s="68"/>
-      <c r="AL1" s="69"/>
-      <c r="AM1" s="67">
+      <c r="AJ1" s="76"/>
+      <c r="AK1" s="76"/>
+      <c r="AL1" s="77"/>
+      <c r="AM1" s="75">
         <v>42087</v>
       </c>
-      <c r="AN1" s="68"/>
-      <c r="AO1" s="68"/>
-      <c r="AP1" s="69"/>
-      <c r="AQ1" s="67">
+      <c r="AN1" s="76"/>
+      <c r="AO1" s="76"/>
+      <c r="AP1" s="77"/>
+      <c r="AQ1" s="75">
         <v>42115</v>
       </c>
-      <c r="AR1" s="68"/>
-      <c r="AS1" s="68"/>
-      <c r="AT1" s="69"/>
-      <c r="AU1" s="67">
+      <c r="AR1" s="76"/>
+      <c r="AS1" s="76"/>
+      <c r="AT1" s="77"/>
+      <c r="AU1" s="75">
         <v>42122</v>
       </c>
-      <c r="AV1" s="68"/>
-      <c r="AW1" s="68"/>
-      <c r="AX1" s="69"/>
-      <c r="AY1" s="67">
+      <c r="AV1" s="76"/>
+      <c r="AW1" s="76"/>
+      <c r="AX1" s="77"/>
+      <c r="AY1" s="75">
         <v>42129</v>
       </c>
-      <c r="AZ1" s="68"/>
-      <c r="BA1" s="68"/>
-      <c r="BB1" s="69"/>
-      <c r="BC1" s="67">
+      <c r="AZ1" s="76"/>
+      <c r="BA1" s="76"/>
+      <c r="BB1" s="77"/>
+      <c r="BC1" s="75">
         <v>42136</v>
       </c>
-      <c r="BD1" s="68"/>
-      <c r="BE1" s="68"/>
-      <c r="BF1" s="69"/>
-      <c r="BG1" s="67">
+      <c r="BD1" s="76"/>
+      <c r="BE1" s="76"/>
+      <c r="BF1" s="77"/>
+      <c r="BG1" s="75">
         <v>42143</v>
       </c>
-      <c r="BH1" s="68"/>
-      <c r="BI1" s="68"/>
-      <c r="BJ1" s="69"/>
-      <c r="BK1" s="67">
+      <c r="BH1" s="76"/>
+      <c r="BI1" s="76"/>
+      <c r="BJ1" s="77"/>
+      <c r="BK1" s="75">
         <v>42150</v>
       </c>
-      <c r="BL1" s="68"/>
-      <c r="BM1" s="68"/>
-      <c r="BN1" s="69"/>
-      <c r="BO1" s="67">
+      <c r="BL1" s="76"/>
+      <c r="BM1" s="76"/>
+      <c r="BN1" s="77"/>
+      <c r="BO1" s="75">
         <v>42157</v>
       </c>
-      <c r="BP1" s="68"/>
-      <c r="BQ1" s="68"/>
-      <c r="BR1" s="69"/>
+      <c r="BP1" s="76"/>
+      <c r="BQ1" s="76"/>
+      <c r="BR1" s="77"/>
       <c r="BS1" s="9"/>
     </row>
-    <row r="2" spans="1:73" s="1" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="70"/>
+    <row r="2" spans="1:73" s="1" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A2" s="89"/>
       <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
@@ -1738,18 +1738,18 @@
       <c r="BT2" s="4"/>
       <c r="BU2" s="4"/>
     </row>
-    <row r="3" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="66">
         <v>1</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="78" t="s">
         <v>37</v>
       </c>
       <c r="C3" s="59"/>
-      <c r="D3" s="77">
+      <c r="D3" s="67">
         <v>4</v>
       </c>
-      <c r="E3" s="77"/>
+      <c r="E3" s="67"/>
       <c r="F3" s="38" t="s">
         <v>1</v>
       </c>
@@ -1791,12 +1791,12 @@
       <c r="BR3" s="12"/>
       <c r="BS3" s="10"/>
     </row>
-    <row r="4" spans="1:73" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:73" s="16" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="66"/>
-      <c r="B4" s="80"/>
+      <c r="B4" s="79"/>
       <c r="C4" s="60"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
       <c r="F4" s="39" t="s">
         <v>2</v>
       </c>
@@ -1870,20 +1870,20 @@
       <c r="BR4" s="15"/>
       <c r="BS4" s="13"/>
     </row>
-    <row r="5" spans="1:73" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:73" s="18" customFormat="1">
       <c r="A5" s="66">
         <v>2</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="72" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="81">
+      <c r="D5" s="74">
         <v>4</v>
       </c>
-      <c r="E5" s="71"/>
+      <c r="E5" s="72"/>
       <c r="F5" s="31" t="s">
         <v>1</v>
       </c>
@@ -1926,12 +1926,12 @@
       <c r="BR5" s="19"/>
       <c r="BS5" s="17"/>
     </row>
-    <row r="6" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:73" s="23" customFormat="1">
       <c r="A6" s="66"/>
-      <c r="B6" s="72"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="63"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
       <c r="F6" s="32" t="s">
         <v>2</v>
       </c>
@@ -2005,20 +2005,20 @@
       <c r="BR6" s="22"/>
       <c r="BS6" s="20"/>
     </row>
-    <row r="7" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="66">
         <v>3</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="67" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="83">
+      <c r="D7" s="69">
         <v>4</v>
       </c>
-      <c r="E7" s="84"/>
+      <c r="E7" s="70"/>
       <c r="F7" s="29" t="s">
         <v>1</v>
       </c>
@@ -2061,12 +2061,12 @@
       <c r="BR7" s="12"/>
       <c r="BS7" s="10"/>
     </row>
-    <row r="8" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:73" s="16" customFormat="1">
       <c r="A8" s="66"/>
-      <c r="B8" s="78"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="56"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="85"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="71"/>
       <c r="F8" s="30" t="s">
         <v>2</v>
       </c>
@@ -2142,20 +2142,20 @@
       <c r="BR8" s="15"/>
       <c r="BS8" s="13"/>
     </row>
-    <row r="9" spans="1:73" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:73" s="18" customFormat="1">
       <c r="A9" s="66">
         <v>7</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="72" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="81">
+      <c r="D9" s="74">
         <v>6</v>
       </c>
-      <c r="E9" s="71"/>
+      <c r="E9" s="72"/>
       <c r="F9" s="31" t="s">
         <v>1</v>
       </c>
@@ -2200,12 +2200,12 @@
       <c r="BR9" s="19"/>
       <c r="BS9" s="17"/>
     </row>
-    <row r="10" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:73" s="23" customFormat="1">
       <c r="A10" s="66"/>
-      <c r="B10" s="72"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="58"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
       <c r="F10" s="32" t="s">
         <v>2</v>
       </c>
@@ -2281,18 +2281,18 @@
       <c r="BR10" s="22"/>
       <c r="BS10" s="20"/>
     </row>
-    <row r="11" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="66">
         <v>4</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="67" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="65"/>
-      <c r="D11" s="83">
-        <v>1</v>
-      </c>
-      <c r="E11" s="84"/>
+      <c r="D11" s="69">
+        <v>1</v>
+      </c>
+      <c r="E11" s="70"/>
       <c r="F11" s="29" t="s">
         <v>1</v>
       </c>
@@ -2333,12 +2333,12 @@
       <c r="BR11" s="12"/>
       <c r="BS11" s="10"/>
     </row>
-    <row r="12" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:73" s="16" customFormat="1">
       <c r="A12" s="66"/>
-      <c r="B12" s="78"/>
+      <c r="B12" s="68"/>
       <c r="C12" s="56"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="85"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="71"/>
       <c r="F12" s="30" t="s">
         <v>2</v>
       </c>
@@ -2410,20 +2410,20 @@
       <c r="BR12" s="15"/>
       <c r="BS12" s="13"/>
     </row>
-    <row r="13" spans="1:73" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:73" s="18" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="66">
         <v>5</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="72" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="71">
+      <c r="D13" s="72">
         <v>4</v>
       </c>
-      <c r="E13" s="71"/>
+      <c r="E13" s="72"/>
       <c r="F13" s="31" t="s">
         <v>1</v>
       </c>
@@ -2466,12 +2466,12 @@
       <c r="BR13" s="19"/>
       <c r="BS13" s="17"/>
     </row>
-    <row r="14" spans="1:73" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:73" s="23" customFormat="1">
       <c r="A14" s="66"/>
-      <c r="B14" s="86"/>
+      <c r="B14" s="84"/>
       <c r="C14" s="64"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
       <c r="F14" s="32" t="s">
         <v>2</v>
       </c>
@@ -2545,20 +2545,20 @@
       <c r="BR14" s="22"/>
       <c r="BS14" s="20"/>
     </row>
-    <row r="15" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:73" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="66">
         <v>6</v>
       </c>
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="67" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="77">
+      <c r="D15" s="67">
         <v>3</v>
       </c>
-      <c r="E15" s="77"/>
+      <c r="E15" s="67"/>
       <c r="F15" s="29" t="s">
         <v>1</v>
       </c>
@@ -2601,12 +2601,12 @@
       <c r="BR15" s="12"/>
       <c r="BS15" s="10"/>
     </row>
-    <row r="16" spans="1:73" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:73" s="16" customFormat="1">
       <c r="A16" s="66"/>
-      <c r="B16" s="78"/>
+      <c r="B16" s="68"/>
       <c r="C16" s="56"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
       <c r="F16" s="30" t="s">
         <v>2</v>
       </c>
@@ -2682,18 +2682,18 @@
       <c r="BR16" s="15"/>
       <c r="BS16" s="13"/>
     </row>
-    <row r="17" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:71" s="18" customFormat="1">
       <c r="A17" s="66">
         <v>7</v>
       </c>
-      <c r="B17" s="71" t="s">
+      <c r="B17" s="72" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="57"/>
-      <c r="D17" s="81">
+      <c r="D17" s="74">
         <v>4</v>
       </c>
-      <c r="E17" s="71"/>
+      <c r="E17" s="72"/>
       <c r="F17" s="31" t="s">
         <v>1</v>
       </c>
@@ -2736,12 +2736,12 @@
       <c r="BR17" s="19"/>
       <c r="BS17" s="17"/>
     </row>
-    <row r="18" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:71" s="23" customFormat="1">
       <c r="A18" s="66"/>
-      <c r="B18" s="72"/>
+      <c r="B18" s="73"/>
       <c r="C18" s="58"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
       <c r="F18" s="32" t="s">
         <v>2</v>
       </c>
@@ -2771,9 +2771,15 @@
       <c r="AD18" s="22"/>
       <c r="AE18" s="20"/>
       <c r="AF18" s="21"/>
-      <c r="AG18" s="21"/>
-      <c r="AH18" s="22"/>
-      <c r="AI18" s="20"/>
+      <c r="AG18" s="21">
+        <v>2</v>
+      </c>
+      <c r="AH18" s="22">
+        <v>2</v>
+      </c>
+      <c r="AI18" s="20">
+        <v>2</v>
+      </c>
       <c r="AJ18" s="21"/>
       <c r="AK18" s="21"/>
       <c r="AL18" s="22"/>
@@ -2811,7 +2817,7 @@
       <c r="BR18" s="22"/>
       <c r="BS18" s="20"/>
     </row>
-    <row r="19" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:71" s="11" customFormat="1">
       <c r="A19" s="66">
         <v>8</v>
       </c>
@@ -2821,10 +2827,10 @@
       <c r="C19" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="77">
+      <c r="D19" s="67">
         <v>8</v>
       </c>
-      <c r="E19" s="77"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="29" t="s">
         <v>1</v>
       </c>
@@ -2872,14 +2878,14 @@
       <c r="BR19" s="12"/>
       <c r="BS19" s="10"/>
     </row>
-    <row r="20" spans="1:71" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:71" s="16" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="66"/>
       <c r="B20" s="52" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="56"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="78"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
       <c r="F20" s="30" t="s">
         <v>2</v>
       </c>
@@ -2912,10 +2918,18 @@
       <c r="AG20" s="14"/>
       <c r="AH20" s="15"/>
       <c r="AI20" s="13"/>
-      <c r="AJ20" s="14"/>
-      <c r="AK20" s="14"/>
-      <c r="AL20" s="15"/>
-      <c r="AM20" s="13"/>
+      <c r="AJ20" s="14">
+        <v>2</v>
+      </c>
+      <c r="AK20" s="14">
+        <v>2</v>
+      </c>
+      <c r="AL20" s="15">
+        <v>2</v>
+      </c>
+      <c r="AM20" s="13">
+        <v>2</v>
+      </c>
       <c r="AN20" s="14"/>
       <c r="AO20" s="14"/>
       <c r="AP20" s="15"/>
@@ -2949,20 +2963,20 @@
       <c r="BR20" s="15"/>
       <c r="BS20" s="13"/>
     </row>
-    <row r="21" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:71" s="18" customFormat="1">
       <c r="A21" s="66">
         <v>7</v>
       </c>
-      <c r="B21" s="71" t="s">
+      <c r="B21" s="72" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="81">
+      <c r="D21" s="74">
         <v>4</v>
       </c>
-      <c r="E21" s="87"/>
+      <c r="E21" s="80"/>
       <c r="F21" s="31" t="s">
         <v>1</v>
       </c>
@@ -3005,12 +3019,12 @@
       <c r="BR21" s="19"/>
       <c r="BS21" s="17"/>
     </row>
-    <row r="22" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:71" s="23" customFormat="1">
       <c r="A22" s="66"/>
-      <c r="B22" s="72"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="58"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="89"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="82"/>
       <c r="F22" s="32" t="s">
         <v>2</v>
       </c>
@@ -3047,8 +3061,12 @@
       <c r="AK22" s="21"/>
       <c r="AL22" s="22"/>
       <c r="AM22" s="20"/>
-      <c r="AN22" s="21"/>
-      <c r="AO22" s="21"/>
+      <c r="AN22" s="21">
+        <v>2</v>
+      </c>
+      <c r="AO22" s="21">
+        <v>2</v>
+      </c>
       <c r="AP22" s="22"/>
       <c r="AQ22" s="20"/>
       <c r="AR22" s="21"/>
@@ -3080,20 +3098,20 @@
       <c r="BR22" s="22"/>
       <c r="BS22" s="20"/>
     </row>
-    <row r="23" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:71" s="11" customFormat="1">
       <c r="A23" s="66">
         <v>8</v>
       </c>
-      <c r="B23" s="77" t="s">
+      <c r="B23" s="67" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="77">
+      <c r="D23" s="67">
         <v>4</v>
       </c>
-      <c r="E23" s="77"/>
+      <c r="E23" s="67"/>
       <c r="F23" s="29" t="s">
         <v>1</v>
       </c>
@@ -3136,12 +3154,12 @@
       <c r="BR23" s="12"/>
       <c r="BS23" s="10"/>
     </row>
-    <row r="24" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:71" s="16" customFormat="1">
       <c r="A24" s="66"/>
-      <c r="B24" s="78"/>
+      <c r="B24" s="68"/>
       <c r="C24" s="56"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
       <c r="F24" s="30" t="s">
         <v>2</v>
       </c>
@@ -3180,7 +3198,9 @@
       <c r="AM24" s="13"/>
       <c r="AN24" s="14"/>
       <c r="AO24" s="14"/>
-      <c r="AP24" s="15"/>
+      <c r="AP24" s="15">
+        <v>2</v>
+      </c>
       <c r="AQ24" s="13"/>
       <c r="AR24" s="14"/>
       <c r="AS24" s="14"/>
@@ -3211,20 +3231,20 @@
       <c r="BR24" s="15"/>
       <c r="BS24" s="13"/>
     </row>
-    <row r="25" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:71" s="18" customFormat="1">
       <c r="A25" s="66">
         <v>7</v>
       </c>
-      <c r="B25" s="71" t="s">
+      <c r="B25" s="72" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="81">
+      <c r="D25" s="74">
         <v>4</v>
       </c>
-      <c r="E25" s="71"/>
+      <c r="E25" s="72"/>
       <c r="F25" s="31" t="s">
         <v>1</v>
       </c>
@@ -3267,12 +3287,12 @@
       <c r="BR25" s="19"/>
       <c r="BS25" s="17"/>
     </row>
-    <row r="26" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:71" s="23" customFormat="1">
       <c r="A26" s="66"/>
-      <c r="B26" s="72"/>
+      <c r="B26" s="73"/>
       <c r="C26" s="58"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
       <c r="F26" s="32" t="s">
         <v>2</v>
       </c>
@@ -3342,20 +3362,20 @@
       <c r="BR26" s="22"/>
       <c r="BS26" s="20"/>
     </row>
-    <row r="27" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:71" s="11" customFormat="1">
       <c r="A27" s="66">
         <v>8</v>
       </c>
-      <c r="B27" s="77" t="s">
+      <c r="B27" s="67" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="77">
+      <c r="D27" s="67">
         <v>4</v>
       </c>
-      <c r="E27" s="77"/>
+      <c r="E27" s="67"/>
       <c r="F27" s="29" t="s">
         <v>1</v>
       </c>
@@ -3398,12 +3418,12 @@
       <c r="BR27" s="12"/>
       <c r="BS27" s="10"/>
     </row>
-    <row r="28" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:71" s="16" customFormat="1">
       <c r="A28" s="66"/>
-      <c r="B28" s="78"/>
+      <c r="B28" s="68"/>
       <c r="C28" s="56"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="78"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
       <c r="F28" s="30" t="s">
         <v>2</v>
       </c>
@@ -3473,20 +3493,20 @@
       <c r="BR28" s="15"/>
       <c r="BS28" s="13"/>
     </row>
-    <row r="29" spans="1:71" s="18" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:71" s="18" customFormat="1" ht="28">
       <c r="A29" s="66">
         <v>9</v>
       </c>
-      <c r="B29" s="71" t="s">
+      <c r="B29" s="72" t="s">
         <v>51</v>
       </c>
       <c r="C29" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="71">
+      <c r="D29" s="72">
         <v>12</v>
       </c>
-      <c r="E29" s="71"/>
+      <c r="E29" s="72"/>
       <c r="F29" s="31" t="s">
         <v>1</v>
       </c>
@@ -3554,12 +3574,12 @@
       <c r="BR29" s="19"/>
       <c r="BS29" s="17"/>
     </row>
-    <row r="30" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:71" s="23" customFormat="1">
       <c r="A30" s="66"/>
-      <c r="B30" s="72"/>
+      <c r="B30" s="73"/>
       <c r="C30" s="58"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="73"/>
       <c r="F30" s="32" t="s">
         <v>2</v>
       </c>
@@ -3591,10 +3611,18 @@
       <c r="AF30" s="21"/>
       <c r="AG30" s="21"/>
       <c r="AH30" s="22"/>
-      <c r="AI30" s="20"/>
-      <c r="AJ30" s="21"/>
-      <c r="AK30" s="21"/>
-      <c r="AL30" s="22"/>
+      <c r="AI30" s="20">
+        <v>2</v>
+      </c>
+      <c r="AJ30" s="21">
+        <v>2</v>
+      </c>
+      <c r="AK30" s="21">
+        <v>2</v>
+      </c>
+      <c r="AL30" s="22">
+        <v>2</v>
+      </c>
       <c r="AM30" s="20"/>
       <c r="AN30" s="21"/>
       <c r="AO30" s="21"/>
@@ -3629,18 +3657,18 @@
       <c r="BR30" s="22"/>
       <c r="BS30" s="20"/>
     </row>
-    <row r="31" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:71" s="11" customFormat="1">
       <c r="A31" s="66">
         <v>10</v>
       </c>
-      <c r="B31" s="77" t="s">
+      <c r="B31" s="67" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="55"/>
-      <c r="D31" s="77">
+      <c r="D31" s="67">
         <v>8</v>
       </c>
-      <c r="E31" s="77"/>
+      <c r="E31" s="67"/>
       <c r="F31" s="29" t="s">
         <v>1</v>
       </c>
@@ -3688,12 +3716,12 @@
       <c r="BR31" s="12"/>
       <c r="BS31" s="10"/>
     </row>
-    <row r="32" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:71" s="16" customFormat="1">
       <c r="A32" s="66"/>
-      <c r="B32" s="78"/>
+      <c r="B32" s="68"/>
       <c r="C32" s="56"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="78"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
       <c r="F32" s="30" t="s">
         <v>2</v>
       </c>
@@ -3732,7 +3760,9 @@
       <c r="AM32" s="13"/>
       <c r="AN32" s="14"/>
       <c r="AO32" s="14"/>
-      <c r="AP32" s="15"/>
+      <c r="AP32" s="15">
+        <v>2</v>
+      </c>
       <c r="AQ32" s="13"/>
       <c r="AR32" s="14"/>
       <c r="AS32" s="14"/>
@@ -3763,18 +3793,18 @@
       <c r="BR32" s="15"/>
       <c r="BS32" s="13"/>
     </row>
-    <row r="33" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:71" s="18" customFormat="1">
       <c r="A33" s="66">
         <v>11</v>
       </c>
-      <c r="B33" s="71" t="s">
+      <c r="B33" s="72" t="s">
         <v>24</v>
       </c>
       <c r="C33" s="57"/>
-      <c r="D33" s="71">
+      <c r="D33" s="72">
         <v>8</v>
       </c>
-      <c r="E33" s="71"/>
+      <c r="E33" s="72"/>
       <c r="F33" s="31" t="s">
         <v>1</v>
       </c>
@@ -3862,12 +3892,12 @@
       <c r="BR33" s="19"/>
       <c r="BS33" s="17"/>
     </row>
-    <row r="34" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:71" s="23" customFormat="1">
       <c r="A34" s="66"/>
-      <c r="B34" s="72"/>
+      <c r="B34" s="73"/>
       <c r="C34" s="58"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
       <c r="F34" s="32" t="s">
         <v>2</v>
       </c>
@@ -3937,18 +3967,18 @@
       <c r="BR34" s="22"/>
       <c r="BS34" s="20"/>
     </row>
-    <row r="35" spans="1:71" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:71" s="11" customFormat="1" ht="17.25" customHeight="1">
       <c r="A35" s="66">
         <v>12</v>
       </c>
-      <c r="B35" s="79" t="s">
+      <c r="B35" s="78" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="59"/>
-      <c r="D35" s="77">
+      <c r="D35" s="67">
         <v>2</v>
       </c>
-      <c r="E35" s="77"/>
+      <c r="E35" s="67"/>
       <c r="F35" s="29" t="s">
         <v>1</v>
       </c>
@@ -3988,12 +4018,12 @@
       <c r="BR35" s="12"/>
       <c r="BS35" s="10"/>
     </row>
-    <row r="36" spans="1:71" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:71" s="16" customFormat="1" ht="15.75" customHeight="1">
       <c r="A36" s="66"/>
-      <c r="B36" s="80"/>
+      <c r="B36" s="79"/>
       <c r="C36" s="60"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="78"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="68"/>
       <c r="F36" s="30" t="s">
         <v>2</v>
       </c>
@@ -4063,18 +4093,18 @@
       <c r="BR36" s="15"/>
       <c r="BS36" s="13"/>
     </row>
-    <row r="37" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:71" s="18" customFormat="1">
       <c r="A37" s="66">
         <v>13</v>
       </c>
-      <c r="B37" s="71" t="s">
+      <c r="B37" s="72" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="57"/>
-      <c r="D37" s="71">
+      <c r="D37" s="72">
         <v>6</v>
       </c>
-      <c r="E37" s="71"/>
+      <c r="E37" s="72"/>
       <c r="F37" s="31" t="s">
         <v>1</v>
       </c>
@@ -4125,12 +4155,12 @@
       <c r="BR37" s="19"/>
       <c r="BS37" s="17"/>
     </row>
-    <row r="38" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:71" s="23" customFormat="1">
       <c r="A38" s="66"/>
-      <c r="B38" s="72"/>
+      <c r="B38" s="73"/>
       <c r="C38" s="58"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="72"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
       <c r="F38" s="32" t="s">
         <v>2</v>
       </c>
@@ -4200,18 +4230,18 @@
       <c r="BR38" s="22"/>
       <c r="BS38" s="20"/>
     </row>
-    <row r="39" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:71" s="11" customFormat="1">
       <c r="A39" s="66">
         <v>14</v>
       </c>
-      <c r="B39" s="77" t="s">
+      <c r="B39" s="67" t="s">
         <v>39</v>
       </c>
       <c r="C39" s="55"/>
-      <c r="D39" s="77">
+      <c r="D39" s="67">
         <v>4</v>
       </c>
-      <c r="E39" s="77"/>
+      <c r="E39" s="67"/>
       <c r="F39" s="29" t="s">
         <v>1</v>
       </c>
@@ -4259,12 +4289,12 @@
       <c r="BR39" s="12"/>
       <c r="BS39" s="10"/>
     </row>
-    <row r="40" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:71" s="16" customFormat="1">
       <c r="A40" s="66"/>
-      <c r="B40" s="78"/>
+      <c r="B40" s="68"/>
       <c r="C40" s="56"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="78"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
       <c r="F40" s="30" t="s">
         <v>2</v>
       </c>
@@ -4334,14 +4364,14 @@
       <c r="BR40" s="15"/>
       <c r="BS40" s="13"/>
     </row>
-    <row r="41" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:71" s="18" customFormat="1">
       <c r="A41" s="66">
         <v>15</v>
       </c>
-      <c r="B41" s="71"/>
+      <c r="B41" s="72"/>
       <c r="C41" s="57"/>
-      <c r="D41" s="71"/>
-      <c r="E41" s="71"/>
+      <c r="D41" s="72"/>
+      <c r="E41" s="72"/>
       <c r="F41" s="31" t="s">
         <v>1</v>
       </c>
@@ -4379,12 +4409,12 @@
       <c r="BR41" s="19"/>
       <c r="BS41" s="17"/>
     </row>
-    <row r="42" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:71" s="23" customFormat="1">
       <c r="A42" s="66"/>
-      <c r="B42" s="72"/>
+      <c r="B42" s="73"/>
       <c r="C42" s="58"/>
-      <c r="D42" s="72"/>
-      <c r="E42" s="72"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="73"/>
       <c r="F42" s="32" t="s">
         <v>2</v>
       </c>
@@ -4454,7 +4484,7 @@
       <c r="BR42" s="22"/>
       <c r="BS42" s="20"/>
     </row>
-    <row r="43" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:71" s="11" customFormat="1">
       <c r="A43" s="66">
         <v>16</v>
       </c>
@@ -4499,7 +4529,7 @@
       <c r="BR43" s="12"/>
       <c r="BS43" s="10"/>
     </row>
-    <row r="44" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:71" s="16" customFormat="1">
       <c r="A44" s="66"/>
       <c r="B44" s="50"/>
       <c r="C44" s="60"/>
@@ -4574,16 +4604,16 @@
       <c r="BR44" s="15"/>
       <c r="BS44" s="13"/>
     </row>
-    <row r="45" spans="1:71" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:71" s="11" customFormat="1" ht="20">
       <c r="A45" s="66">
         <v>18</v>
       </c>
-      <c r="B45" s="73" t="s">
+      <c r="B45" s="85" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="61"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
+      <c r="D45" s="87"/>
+      <c r="E45" s="87"/>
       <c r="F45" s="40"/>
       <c r="G45" s="41"/>
       <c r="H45" s="42"/>
@@ -4671,12 +4701,12 @@
       <c r="BR45" s="43"/>
       <c r="BS45" s="10"/>
     </row>
-    <row r="46" spans="1:71" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:71" s="16" customFormat="1" ht="20">
       <c r="A46" s="66"/>
-      <c r="B46" s="74"/>
+      <c r="B46" s="86"/>
       <c r="C46" s="62"/>
-      <c r="D46" s="76"/>
-      <c r="E46" s="76"/>
+      <c r="D46" s="88"/>
+      <c r="E46" s="88"/>
       <c r="F46" s="44"/>
       <c r="G46" s="45"/>
       <c r="H46" s="46"/>
@@ -4744,16 +4774,16 @@
       <c r="BR46" s="47"/>
       <c r="BS46" s="13"/>
     </row>
-    <row r="47" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:71" s="18" customFormat="1">
       <c r="A47" s="66">
         <v>19</v>
       </c>
-      <c r="B47" s="71" t="s">
+      <c r="B47" s="72" t="s">
         <v>40</v>
       </c>
       <c r="C47" s="57"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="71"/>
+      <c r="D47" s="72"/>
+      <c r="E47" s="72"/>
       <c r="F47" s="31"/>
       <c r="G47" s="17"/>
       <c r="J47" s="19"/>
@@ -4789,12 +4819,12 @@
       <c r="BR47" s="19"/>
       <c r="BS47" s="17"/>
     </row>
-    <row r="48" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:71" s="23" customFormat="1">
       <c r="A48" s="66"/>
-      <c r="B48" s="72"/>
+      <c r="B48" s="73"/>
       <c r="C48" s="58"/>
-      <c r="D48" s="72"/>
-      <c r="E48" s="72"/>
+      <c r="D48" s="73"/>
+      <c r="E48" s="73"/>
       <c r="F48" s="32"/>
       <c r="G48" s="20"/>
       <c r="H48" s="21"/>
@@ -4862,16 +4892,16 @@
       <c r="BR48" s="22"/>
       <c r="BS48" s="20"/>
     </row>
-    <row r="49" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:71" s="11" customFormat="1">
       <c r="A49" s="66">
         <v>20</v>
       </c>
-      <c r="B49" s="77" t="s">
+      <c r="B49" s="67" t="s">
         <v>41</v>
       </c>
       <c r="C49" s="55"/>
-      <c r="D49" s="77"/>
-      <c r="E49" s="77"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="67"/>
       <c r="F49" s="29"/>
       <c r="G49" s="10"/>
       <c r="J49" s="12"/>
@@ -4907,12 +4937,12 @@
       <c r="BR49" s="12"/>
       <c r="BS49" s="10"/>
     </row>
-    <row r="50" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:71" s="16" customFormat="1">
       <c r="A50" s="66"/>
-      <c r="B50" s="78"/>
+      <c r="B50" s="68"/>
       <c r="C50" s="56"/>
-      <c r="D50" s="78"/>
-      <c r="E50" s="78"/>
+      <c r="D50" s="68"/>
+      <c r="E50" s="68"/>
       <c r="F50" s="30"/>
       <c r="G50" s="13"/>
       <c r="H50" s="14"/>
@@ -4980,16 +5010,16 @@
       <c r="BR50" s="15"/>
       <c r="BS50" s="13"/>
     </row>
-    <row r="51" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:71" s="18" customFormat="1">
       <c r="A51" s="66">
         <v>21</v>
       </c>
-      <c r="B51" s="71" t="s">
+      <c r="B51" s="72" t="s">
         <v>42</v>
       </c>
       <c r="C51" s="57"/>
-      <c r="D51" s="71"/>
-      <c r="E51" s="71"/>
+      <c r="D51" s="72"/>
+      <c r="E51" s="72"/>
       <c r="F51" s="31"/>
       <c r="G51" s="17"/>
       <c r="J51" s="19"/>
@@ -5025,12 +5055,12 @@
       <c r="BR51" s="19"/>
       <c r="BS51" s="17"/>
     </row>
-    <row r="52" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:71" s="23" customFormat="1">
       <c r="A52" s="66"/>
-      <c r="B52" s="72"/>
+      <c r="B52" s="73"/>
       <c r="C52" s="58"/>
-      <c r="D52" s="72"/>
-      <c r="E52" s="72"/>
+      <c r="D52" s="73"/>
+      <c r="E52" s="73"/>
       <c r="F52" s="32"/>
       <c r="G52" s="20"/>
       <c r="H52" s="21"/>
@@ -5098,16 +5128,16 @@
       <c r="BR52" s="22"/>
       <c r="BS52" s="20"/>
     </row>
-    <row r="53" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:71" s="11" customFormat="1">
       <c r="A53" s="66">
         <v>22</v>
       </c>
-      <c r="B53" s="77" t="s">
+      <c r="B53" s="67" t="s">
         <v>43</v>
       </c>
       <c r="C53" s="55"/>
-      <c r="D53" s="77"/>
-      <c r="E53" s="77"/>
+      <c r="D53" s="67"/>
+      <c r="E53" s="67"/>
       <c r="F53" s="29"/>
       <c r="G53" s="10"/>
       <c r="J53" s="12"/>
@@ -5143,12 +5173,12 @@
       <c r="BR53" s="12"/>
       <c r="BS53" s="10"/>
     </row>
-    <row r="54" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:71" s="16" customFormat="1">
       <c r="A54" s="66"/>
-      <c r="B54" s="78"/>
+      <c r="B54" s="68"/>
       <c r="C54" s="56"/>
-      <c r="D54" s="78"/>
-      <c r="E54" s="78"/>
+      <c r="D54" s="68"/>
+      <c r="E54" s="68"/>
       <c r="F54" s="30"/>
       <c r="G54" s="13"/>
       <c r="H54" s="14"/>
@@ -5216,16 +5246,16 @@
       <c r="BR54" s="15"/>
       <c r="BS54" s="13"/>
     </row>
-    <row r="55" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:71" s="18" customFormat="1">
       <c r="A55" s="66">
         <v>23</v>
       </c>
-      <c r="B55" s="71" t="s">
+      <c r="B55" s="72" t="s">
         <v>44</v>
       </c>
       <c r="C55" s="57"/>
-      <c r="D55" s="71"/>
-      <c r="E55" s="71"/>
+      <c r="D55" s="72"/>
+      <c r="E55" s="72"/>
       <c r="F55" s="31"/>
       <c r="G55" s="17"/>
       <c r="J55" s="19"/>
@@ -5261,12 +5291,12 @@
       <c r="BR55" s="19"/>
       <c r="BS55" s="17"/>
     </row>
-    <row r="56" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:71" s="23" customFormat="1">
       <c r="A56" s="66"/>
-      <c r="B56" s="72"/>
+      <c r="B56" s="73"/>
       <c r="C56" s="58"/>
-      <c r="D56" s="72"/>
-      <c r="E56" s="72"/>
+      <c r="D56" s="73"/>
+      <c r="E56" s="73"/>
       <c r="F56" s="32"/>
       <c r="G56" s="20"/>
       <c r="H56" s="21"/>
@@ -5334,16 +5364,16 @@
       <c r="BR56" s="22"/>
       <c r="BS56" s="20"/>
     </row>
-    <row r="57" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:71" s="11" customFormat="1">
       <c r="A57" s="66">
         <v>24</v>
       </c>
-      <c r="B57" s="77" t="s">
+      <c r="B57" s="67" t="s">
         <v>45</v>
       </c>
       <c r="C57" s="55"/>
-      <c r="D57" s="77"/>
-      <c r="E57" s="77"/>
+      <c r="D57" s="67"/>
+      <c r="E57" s="67"/>
       <c r="F57" s="29"/>
       <c r="G57" s="10"/>
       <c r="J57" s="12"/>
@@ -5379,12 +5409,12 @@
       <c r="BR57" s="12"/>
       <c r="BS57" s="10"/>
     </row>
-    <row r="58" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:71" s="16" customFormat="1">
       <c r="A58" s="66"/>
-      <c r="B58" s="78"/>
+      <c r="B58" s="68"/>
       <c r="C58" s="56"/>
-      <c r="D58" s="78"/>
-      <c r="E58" s="78"/>
+      <c r="D58" s="68"/>
+      <c r="E58" s="68"/>
       <c r="F58" s="30"/>
       <c r="G58" s="13"/>
       <c r="H58" s="14"/>
@@ -5452,16 +5482,16 @@
       <c r="BR58" s="15"/>
       <c r="BS58" s="13"/>
     </row>
-    <row r="59" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:71" s="18" customFormat="1">
       <c r="A59" s="66">
         <v>25</v>
       </c>
-      <c r="B59" s="71" t="s">
+      <c r="B59" s="72" t="s">
         <v>46</v>
       </c>
       <c r="C59" s="57"/>
-      <c r="D59" s="71"/>
-      <c r="E59" s="71"/>
+      <c r="D59" s="72"/>
+      <c r="E59" s="72"/>
       <c r="F59" s="31"/>
       <c r="G59" s="17"/>
       <c r="J59" s="19"/>
@@ -5497,12 +5527,12 @@
       <c r="BR59" s="19"/>
       <c r="BS59" s="17"/>
     </row>
-    <row r="60" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:71" s="23" customFormat="1">
       <c r="A60" s="66"/>
-      <c r="B60" s="72"/>
+      <c r="B60" s="73"/>
       <c r="C60" s="58"/>
-      <c r="D60" s="72"/>
-      <c r="E60" s="72"/>
+      <c r="D60" s="73"/>
+      <c r="E60" s="73"/>
       <c r="F60" s="32"/>
       <c r="G60" s="20"/>
       <c r="H60" s="21"/>
@@ -5570,16 +5600,16 @@
       <c r="BR60" s="22"/>
       <c r="BS60" s="20"/>
     </row>
-    <row r="61" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:71" s="11" customFormat="1">
       <c r="A61" s="66">
         <v>26</v>
       </c>
-      <c r="B61" s="77" t="s">
+      <c r="B61" s="67" t="s">
         <v>47</v>
       </c>
       <c r="C61" s="55"/>
-      <c r="D61" s="77"/>
-      <c r="E61" s="77"/>
+      <c r="D61" s="67"/>
+      <c r="E61" s="67"/>
       <c r="F61" s="29"/>
       <c r="G61" s="10"/>
       <c r="J61" s="12"/>
@@ -5615,12 +5645,12 @@
       <c r="BR61" s="12"/>
       <c r="BS61" s="10"/>
     </row>
-    <row r="62" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:71" s="16" customFormat="1">
       <c r="A62" s="66"/>
-      <c r="B62" s="78"/>
+      <c r="B62" s="68"/>
       <c r="C62" s="56"/>
-      <c r="D62" s="78"/>
-      <c r="E62" s="78"/>
+      <c r="D62" s="68"/>
+      <c r="E62" s="68"/>
       <c r="F62" s="30"/>
       <c r="G62" s="13"/>
       <c r="H62" s="14"/>
@@ -5688,16 +5718,16 @@
       <c r="BR62" s="15"/>
       <c r="BS62" s="13"/>
     </row>
-    <row r="63" spans="1:71" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:71" s="18" customFormat="1">
       <c r="A63" s="66">
         <v>27</v>
       </c>
-      <c r="B63" s="71" t="s">
+      <c r="B63" s="72" t="s">
         <v>48</v>
       </c>
       <c r="C63" s="57"/>
-      <c r="D63" s="71"/>
-      <c r="E63" s="71"/>
+      <c r="D63" s="72"/>
+      <c r="E63" s="72"/>
       <c r="F63" s="31"/>
       <c r="G63" s="17"/>
       <c r="J63" s="19"/>
@@ -5733,12 +5763,12 @@
       <c r="BR63" s="19"/>
       <c r="BS63" s="17"/>
     </row>
-    <row r="64" spans="1:71" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:71" s="23" customFormat="1">
       <c r="A64" s="66"/>
-      <c r="B64" s="72"/>
+      <c r="B64" s="73"/>
       <c r="C64" s="58"/>
-      <c r="D64" s="72"/>
-      <c r="E64" s="72"/>
+      <c r="D64" s="73"/>
+      <c r="E64" s="73"/>
       <c r="F64" s="32"/>
       <c r="G64" s="20"/>
       <c r="H64" s="21"/>
@@ -5806,16 +5836,16 @@
       <c r="BR64" s="22"/>
       <c r="BS64" s="20"/>
     </row>
-    <row r="65" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:71" s="11" customFormat="1">
       <c r="A65" s="66">
         <v>28</v>
       </c>
-      <c r="B65" s="77" t="s">
+      <c r="B65" s="67" t="s">
         <v>49</v>
       </c>
       <c r="C65" s="55"/>
-      <c r="D65" s="77"/>
-      <c r="E65" s="77"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="67"/>
       <c r="F65" s="29"/>
       <c r="G65" s="10"/>
       <c r="J65" s="12"/>
@@ -5851,12 +5881,12 @@
       <c r="BR65" s="12"/>
       <c r="BS65" s="10"/>
     </row>
-    <row r="66" spans="1:71" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:71" s="16" customFormat="1">
       <c r="A66" s="66"/>
-      <c r="B66" s="78"/>
+      <c r="B66" s="68"/>
       <c r="C66" s="56"/>
-      <c r="D66" s="78"/>
-      <c r="E66" s="78"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="68"/>
       <c r="F66" s="33"/>
       <c r="G66" s="13"/>
       <c r="H66" s="14"/>
@@ -5924,7 +5954,7 @@
       <c r="BR66" s="15"/>
       <c r="BS66" s="13"/>
     </row>
-    <row r="67" spans="1:71" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:71">
       <c r="B67" s="6" t="s">
         <v>12</v>
       </c>
@@ -5934,26 +5964,72 @@
     </row>
   </sheetData>
   <mergeCells count="110">
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:E50"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:E8"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="D27:E28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D29:E30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="D31:E32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="D17:E18"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="AQ1:AT1"/>
+    <mergeCell ref="AU1:AX1"/>
+    <mergeCell ref="AY1:BB1"/>
+    <mergeCell ref="BO1:BR1"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AM1:AP1"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="AA1:AD1"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="D63:E64"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D45:E46"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="D65:E66"/>
+    <mergeCell ref="D51:E52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:E54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="D55:E56"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="D57:E58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="D59:E60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="D61:E62"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:E24"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:E10"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="D41:E42"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D25:E26"/>
     <mergeCell ref="BC1:BF1"/>
     <mergeCell ref="BG1:BJ1"/>
     <mergeCell ref="BK1:BN1"/>
@@ -5978,72 +6054,26 @@
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="D21:E22"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:E24"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:E10"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="D41:E42"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:E6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:E12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D13:E14"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D25:E26"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="D63:E64"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D45:E46"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="D65:E66"/>
-    <mergeCell ref="D51:E52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:E54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="D55:E56"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="D57:E58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="D59:E60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="D61:E62"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="AQ1:AT1"/>
-    <mergeCell ref="AU1:AX1"/>
-    <mergeCell ref="AY1:BB1"/>
-    <mergeCell ref="BO1:BR1"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AM1:AP1"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="AA1:AD1"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:E50"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D27:E28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D29:E30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="D31:E32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="D17:E18"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:BR8 G25:BR44 G11:BR16 G46:BR64 G45:AW45 BD45:BR45 AY45:BB45">
     <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
@@ -6094,7 +6124,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>